<commit_message>
updated sex and age specific table for prevalence of CAG
</commit_message>
<xml_diff>
--- a/docs/source/concept_models/vivarium_swissre_stomachcancer/precancer_states_and_hpylori_memo_28dec2020.xlsx
+++ b/docs/source/concept_models/vivarium_swissre_stomachcancer/precancer_states_and_hpylori_memo_28dec2020.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="120">
   <si>
     <t>Male</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>% H+</t>
+  </si>
+  <si>
+    <t>RR of CAG among H+</t>
   </si>
 </sst>
 </file>
@@ -877,7 +880,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1212,6 +1215,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,25 +1342,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1388,23 +1391,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="7" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1414,6 +1423,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6589,15 +6603,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>195263</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>338138</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>366082</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>73145</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>318457</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1707</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6614,7 +6628,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7398544" y="4826793"/>
+          <a:off x="7255669" y="7243762"/>
           <a:ext cx="5028569" cy="5402383"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6953,12 +6967,12 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -8037,16 +8051,16 @@
       <c r="E2" s="59">
         <v>1000</v>
       </c>
-      <c r="N2" s="136" t="s">
+      <c r="N2" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="136"/>
-      <c r="S2" s="136"/>
-      <c r="T2" s="136"/>
-      <c r="U2" s="136"/>
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="137"/>
+      <c r="T2" s="137"/>
+      <c r="U2" s="137"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="61" t="s">
@@ -8067,10 +8081,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="72"/>
-      <c r="G4" s="154" t="s">
+      <c r="G4" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="154"/>
+      <c r="H4" s="155"/>
       <c r="I4" s="94" t="s">
         <v>6</v>
       </c>
@@ -8087,10 +8101,10 @@
         <v>2</v>
       </c>
       <c r="O4" s="115"/>
-      <c r="P4" s="137" t="s">
+      <c r="P4" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="137"/>
+      <c r="Q4" s="138"/>
       <c r="R4" s="116" t="s">
         <v>6</v>
       </c>
@@ -8115,7 +8129,7 @@
       <c r="AB4" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="133"/>
+      <c r="AC4" s="134"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
@@ -8127,17 +8141,17 @@
       <c r="D5" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="138" t="s">
+      <c r="E5" s="139" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="153">
+      <c r="G5" s="154">
         <f>L5-K5-J5-I5</f>
         <v>309.5</v>
       </c>
-      <c r="H5" s="153"/>
+      <c r="H5" s="154"/>
       <c r="I5" s="82">
         <f>I9*I7</f>
         <v>162.5</v>
@@ -8153,47 +8167,47 @@
       <c r="L5" s="98">
         <v>550</v>
       </c>
-      <c r="N5" s="138" t="s">
+      <c r="N5" s="139" t="s">
         <v>33</v>
       </c>
       <c r="O5" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="144">
+      <c r="P5" s="145">
         <f>(G7*G9/1000)/0.55</f>
         <v>0.56272727272727263</v>
       </c>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="122">
+      <c r="Q5" s="145"/>
+      <c r="R5" s="123">
         <f>(I7*I9/1000)/0.55</f>
         <v>0.29545454545454541</v>
       </c>
-      <c r="S5" s="122">
+      <c r="S5" s="123">
         <f>(J7*J9/1000)/0.55</f>
         <v>0.14181818181818182</v>
       </c>
-      <c r="T5" s="122">
+      <c r="T5" s="123">
         <f>(K7*K9/1000)/0.55</f>
         <v>0</v>
       </c>
-      <c r="U5" s="124">
+      <c r="U5" s="125">
         <f>SUM(P5:T5)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="W5" s="131" t="s">
+      <c r="W5" s="132" t="s">
         <v>33</v>
       </c>
       <c r="X5" s="81"/>
-      <c r="Y5" s="134">
+      <c r="Y5" s="135">
         <v>0.42699999999999999</v>
       </c>
-      <c r="Z5" s="134">
+      <c r="Z5" s="135">
         <v>0.45864045864045866</v>
       </c>
-      <c r="AA5" s="134">
+      <c r="AA5" s="135">
         <v>0.2424242424242424</v>
       </c>
-      <c r="AB5" s="134">
+      <c r="AB5" s="135">
         <v>1.6380016380015937E-3</v>
       </c>
       <c r="AC5" s="75"/>
@@ -8204,15 +8218,15 @@
         <v>26</v>
       </c>
       <c r="D6" s="97"/>
-      <c r="E6" s="139"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="142">
+      <c r="G6" s="143">
         <f>G7-G5</f>
         <v>340.5</v>
       </c>
-      <c r="H6" s="142"/>
+      <c r="H6" s="143"/>
       <c r="I6" s="84">
         <f t="shared" ref="I6:J6" si="1">I7-I5</f>
         <v>87.5</v>
@@ -8228,14 +8242,14 @@
       <c r="L6" s="99">
         <v>450</v>
       </c>
-      <c r="N6" s="139"/>
+      <c r="N6" s="140"/>
       <c r="O6" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="142" t="s">
+      <c r="P6" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="142"/>
+      <c r="Q6" s="143"/>
       <c r="R6" s="84" t="s">
         <v>52</v>
       </c>
@@ -8270,15 +8284,15 @@
         <v>27</v>
       </c>
       <c r="D7" s="48"/>
-      <c r="E7" s="139"/>
+      <c r="E7" s="140"/>
       <c r="F7" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="147">
+      <c r="G7" s="148">
         <f>((G36+H36)/(1-L36))*$E$2</f>
         <v>650</v>
       </c>
-      <c r="H7" s="147"/>
+      <c r="H7" s="148"/>
       <c r="I7" s="87">
         <f>(I36/(1-L36))*$E$2</f>
         <v>250</v>
@@ -8295,17 +8309,17 @@
         <f>SUM(G7:K7)</f>
         <v>1000</v>
       </c>
-      <c r="N7" s="140"/>
-      <c r="O7" s="118" t="s">
+      <c r="N7" s="141"/>
+      <c r="O7" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="119"/>
-      <c r="S7" s="119"/>
-      <c r="T7" s="119"/>
-      <c r="U7" s="120"/>
-      <c r="W7" s="132" t="s">
+      <c r="P7" s="144"/>
+      <c r="Q7" s="144"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
+      <c r="T7" s="120"/>
+      <c r="U7" s="121"/>
+      <c r="W7" s="133" t="s">
         <v>92</v>
       </c>
       <c r="Y7" s="58">
@@ -8331,11 +8345,11 @@
       <c r="F8" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="148">
+      <c r="G8" s="149">
         <f>G7/$L$7</f>
         <v>0.65</v>
       </c>
-      <c r="H8" s="148"/>
+      <c r="H8" s="149"/>
       <c r="I8" s="112">
         <f t="shared" ref="I8:L8" si="2">I7/$L$7</f>
         <v>0.25</v>
@@ -8378,18 +8392,18 @@
       <c r="F9" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="152">
+      <c r="G9" s="153">
         <f>G5/G7</f>
         <v>0.47615384615384615</v>
       </c>
-      <c r="H9" s="152"/>
-      <c r="I9" s="123">
+      <c r="H9" s="153"/>
+      <c r="I9" s="124">
         <v>0.65</v>
       </c>
-      <c r="J9" s="123">
+      <c r="J9" s="124">
         <v>0.78</v>
       </c>
-      <c r="K9" s="123">
+      <c r="K9" s="124">
         <v>0.78</v>
       </c>
       <c r="L9" s="102"/>
@@ -8423,17 +8437,17 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D11" s="97"/>
-      <c r="E11" s="138" t="s">
+      <c r="E11" s="139" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="153">
+      <c r="G11" s="154">
         <f>L11-K11-J11-I11</f>
         <v>251.48148148148147</v>
       </c>
-      <c r="H11" s="153"/>
+      <c r="H11" s="154"/>
       <c r="I11" s="82">
         <f>I15*I13</f>
         <v>182.1821821821822</v>
@@ -8453,10 +8467,10 @@
         <v>2</v>
       </c>
       <c r="O11" s="115"/>
-      <c r="P11" s="137" t="s">
+      <c r="P11" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" s="137"/>
+      <c r="Q11" s="138"/>
       <c r="R11" s="116" t="s">
         <v>6</v>
       </c>
@@ -8471,15 +8485,15 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D12" s="97"/>
-      <c r="E12" s="139"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="142">
+      <c r="G12" s="143">
         <f>G13-G11</f>
         <v>319.08908908908899</v>
       </c>
-      <c r="H12" s="142"/>
+      <c r="H12" s="143"/>
       <c r="I12" s="84">
         <f t="shared" ref="I12" si="4">I13-I11</f>
         <v>98.098098098098092</v>
@@ -8495,30 +8509,30 @@
       <c r="L12" s="99">
         <v>450</v>
       </c>
-      <c r="N12" s="138" t="s">
+      <c r="N12" s="139" t="s">
         <v>34</v>
       </c>
       <c r="O12" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="144">
+      <c r="P12" s="145">
         <f>(G13*G15/1000)/0.55</f>
         <v>0.30084630084630076</v>
       </c>
-      <c r="Q12" s="144"/>
-      <c r="R12" s="122">
+      <c r="Q12" s="145"/>
+      <c r="R12" s="123">
         <f>(I13*I15/1000)/0.55</f>
         <v>0.33124033124033125</v>
       </c>
-      <c r="S12" s="122">
+      <c r="S12" s="123">
         <f>(J13*J15/1000)/0.55</f>
         <v>0.21010101010101007</v>
       </c>
-      <c r="T12" s="122">
+      <c r="T12" s="123">
         <f>(K13*K15/1000)/0.55</f>
         <v>1.4196014196013811E-3</v>
       </c>
-      <c r="U12" s="124">
+      <c r="U12" s="125">
         <f>SUM(P12:T12)</f>
         <v>0.8436072436072436</v>
       </c>
@@ -8526,15 +8540,15 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D13" s="97"/>
-      <c r="E13" s="139"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="147">
+      <c r="G13" s="148">
         <f>((G37+H37)/(1-L37))*$E$2</f>
         <v>570.57057057057045</v>
       </c>
-      <c r="H13" s="147"/>
+      <c r="H13" s="148"/>
       <c r="I13" s="87">
         <f>(I37/(1-L37))*$E$2</f>
         <v>280.28028028028029</v>
@@ -8551,14 +8565,14 @@
         <f>SUM(G13:K13)</f>
         <v>999.99999999999989</v>
       </c>
-      <c r="N13" s="139"/>
+      <c r="N13" s="140"/>
       <c r="O13" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="142" t="s">
+      <c r="P13" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="Q13" s="142"/>
+      <c r="Q13" s="143"/>
       <c r="R13" s="84" t="s">
         <v>52</v>
       </c>
@@ -8579,11 +8593,11 @@
       <c r="F14" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="148">
+      <c r="G14" s="149">
         <f>G13/$L$7</f>
         <v>0.57057057057057048</v>
       </c>
-      <c r="H14" s="148"/>
+      <c r="H14" s="149"/>
       <c r="I14" s="112">
         <f t="shared" ref="I14" si="6">I13/$L$7</f>
         <v>0.28028028028028029</v>
@@ -8600,16 +8614,16 @@
         <f>SUM(G14:K14)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="N14" s="140"/>
-      <c r="O14" s="118" t="s">
+      <c r="N14" s="141"/>
+      <c r="O14" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="P14" s="143"/>
-      <c r="Q14" s="143"/>
-      <c r="R14" s="119"/>
-      <c r="S14" s="119"/>
-      <c r="T14" s="119"/>
-      <c r="U14" s="120"/>
+      <c r="P14" s="144"/>
+      <c r="Q14" s="144"/>
+      <c r="R14" s="120"/>
+      <c r="S14" s="120"/>
+      <c r="T14" s="120"/>
+      <c r="U14" s="121"/>
       <c r="Y14" s="27"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -8618,17 +8632,17 @@
       <c r="F15" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="152">
+      <c r="G15" s="153">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H15" s="152"/>
-      <c r="I15" s="123">
+      <c r="H15" s="153"/>
+      <c r="I15" s="124">
         <v>0.65</v>
       </c>
-      <c r="J15" s="123">
+      <c r="J15" s="124">
         <v>0.78</v>
       </c>
-      <c r="K15" s="123">
+      <c r="K15" s="124">
         <v>0.78</v>
       </c>
       <c r="L15" s="102"/>
@@ -8649,17 +8663,17 @@
     </row>
     <row r="17" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D17" s="97"/>
-      <c r="E17" s="138" t="s">
+      <c r="E17" s="139" t="s">
         <v>35</v>
       </c>
       <c r="F17" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="153">
+      <c r="G17" s="154">
         <f>L17-K17-J17-I17</f>
         <v>179.42828485456371</v>
       </c>
-      <c r="H17" s="153"/>
+      <c r="H17" s="154"/>
       <c r="I17" s="82">
         <f>I21*I19</f>
         <v>208.62587763289869</v>
@@ -8679,10 +8693,10 @@
         <v>2</v>
       </c>
       <c r="O17" s="115"/>
-      <c r="P17" s="137" t="s">
+      <c r="P17" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="137"/>
+      <c r="Q17" s="138"/>
       <c r="R17" s="116" t="s">
         <v>6</v>
       </c>
@@ -8699,15 +8713,15 @@
     </row>
     <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="48"/>
-      <c r="E18" s="139"/>
+      <c r="E18" s="140"/>
       <c r="F18" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="142">
+      <c r="G18" s="143">
         <f>G19-G17</f>
         <v>291.98595787362081</v>
       </c>
-      <c r="H18" s="142"/>
+      <c r="H18" s="143"/>
       <c r="I18" s="84">
         <f t="shared" ref="I18" si="10">I19-I17</f>
         <v>112.33701103309929</v>
@@ -8723,45 +8737,45 @@
       <c r="L18" s="99">
         <v>450</v>
       </c>
-      <c r="N18" s="138" t="s">
+      <c r="N18" s="139" t="s">
         <v>35</v>
       </c>
       <c r="O18" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P18" s="141">
+      <c r="P18" s="142">
         <f>(G19*G21/1000)/0.55</f>
         <v>0.32623324519011582</v>
       </c>
-      <c r="Q18" s="141"/>
-      <c r="R18" s="121">
+      <c r="Q18" s="142"/>
+      <c r="R18" s="122">
         <f>(I19*I21/1000)/0.55</f>
         <v>0.37931977751436124</v>
       </c>
-      <c r="S18" s="121">
+      <c r="S18" s="122">
         <f>(J19*J21/1000)/0.55</f>
         <v>0.28448983313577098</v>
       </c>
-      <c r="T18" s="121">
+      <c r="T18" s="122">
         <f>(K19*K21/1000)/0.55</f>
         <v>9.9571441597518951E-3</v>
       </c>
-      <c r="U18" s="124">
+      <c r="U18" s="125">
         <f>SUM(P18:T18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="48"/>
-      <c r="E19" s="139"/>
+      <c r="E19" s="140"/>
       <c r="F19" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="147">
+      <c r="G19" s="148">
         <f>((G38+H38)/(1-L38))*$E$2</f>
         <v>471.41424272818455</v>
       </c>
-      <c r="H19" s="147"/>
+      <c r="H19" s="148"/>
       <c r="I19" s="87">
         <f>(I38/(1-L38))*$E$2</f>
         <v>320.96288866599798</v>
@@ -8778,14 +8792,14 @@
         <f>SUM(G19:K19)</f>
         <v>999.99999999999989</v>
       </c>
-      <c r="N19" s="139"/>
+      <c r="N19" s="140"/>
       <c r="O19" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="142" t="s">
+      <c r="P19" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" s="142"/>
+      <c r="Q19" s="143"/>
       <c r="R19" s="84" t="s">
         <v>52</v>
       </c>
@@ -8805,11 +8819,11 @@
       <c r="F20" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="148">
+      <c r="G20" s="149">
         <f>G19/$L$7</f>
         <v>0.47141424272818455</v>
       </c>
-      <c r="H20" s="148"/>
+      <c r="H20" s="149"/>
       <c r="I20" s="112">
         <f t="shared" ref="I20" si="12">I19/$L$7</f>
         <v>0.32096288866599798</v>
@@ -8826,16 +8840,16 @@
         <f>SUM(G20:K20)</f>
         <v>1</v>
       </c>
-      <c r="N20" s="140"/>
-      <c r="O20" s="118" t="s">
+      <c r="N20" s="141"/>
+      <c r="O20" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="P20" s="143"/>
-      <c r="Q20" s="143"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="119"/>
-      <c r="T20" s="119"/>
-      <c r="U20" s="120"/>
+      <c r="P20" s="144"/>
+      <c r="Q20" s="144"/>
+      <c r="R20" s="120"/>
+      <c r="S20" s="120"/>
+      <c r="T20" s="120"/>
+      <c r="U20" s="121"/>
     </row>
     <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="48"/>
@@ -8843,18 +8857,18 @@
       <c r="F21" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="152">
+      <c r="G21" s="153">
         <f>G17/G19</f>
         <v>0.3806170212765958</v>
       </c>
-      <c r="H21" s="152"/>
-      <c r="I21" s="123">
+      <c r="H21" s="153"/>
+      <c r="I21" s="124">
         <v>0.65</v>
       </c>
-      <c r="J21" s="123">
+      <c r="J21" s="124">
         <v>0.78</v>
       </c>
-      <c r="K21" s="123">
+      <c r="K21" s="124">
         <v>0.78</v>
       </c>
       <c r="L21" s="102"/>
@@ -8872,17 +8886,17 @@
     </row>
     <row r="23" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D23" s="48"/>
-      <c r="E23" s="150" t="s">
+      <c r="E23" s="151" t="s">
         <v>36</v>
       </c>
       <c r="F23" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="153">
+      <c r="G23" s="154">
         <f>L23-K23-J23-I23</f>
         <v>150.20100502512565</v>
       </c>
-      <c r="H23" s="153"/>
+      <c r="H23" s="154"/>
       <c r="I23" s="82">
         <f>I27*I25</f>
         <v>215.5778894472362</v>
@@ -8902,10 +8916,10 @@
         <v>2</v>
       </c>
       <c r="O23" s="115"/>
-      <c r="P23" s="137" t="s">
+      <c r="P23" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="Q23" s="137"/>
+      <c r="Q23" s="138"/>
       <c r="R23" s="116" t="s">
         <v>6</v>
       </c>
@@ -8919,15 +8933,15 @@
     </row>
     <row r="24" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D24" s="48"/>
-      <c r="E24" s="151"/>
+      <c r="E24" s="152"/>
       <c r="F24" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="142">
+      <c r="G24" s="143">
         <f>G25-G23</f>
         <v>281.95979899497485</v>
       </c>
-      <c r="H24" s="142"/>
+      <c r="H24" s="143"/>
       <c r="I24" s="84">
         <f t="shared" ref="I24" si="16">I25-I23</f>
         <v>116.08040201005025</v>
@@ -8943,45 +8957,45 @@
       <c r="L24" s="99">
         <v>450</v>
       </c>
-      <c r="N24" s="138" t="s">
+      <c r="N24" s="139" t="s">
         <v>36</v>
       </c>
       <c r="O24" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P24" s="141">
+      <c r="P24" s="142">
         <f>(G25*G27/1000)/0.55</f>
         <v>0.27309273640931936</v>
       </c>
-      <c r="Q24" s="141"/>
-      <c r="R24" s="121">
+      <c r="Q24" s="142"/>
+      <c r="R24" s="122">
         <f>(I25*I27/1000)/0.55</f>
         <v>0.39195979899497491</v>
       </c>
-      <c r="S24" s="121">
+      <c r="S24" s="122">
         <f>(J25*J27/1000)/0.55</f>
         <v>0.32782092279579716</v>
       </c>
-      <c r="T24" s="121">
+      <c r="T24" s="122">
         <f>(K25*K27/1000)/0.55</f>
         <v>7.1265417999086108E-3</v>
       </c>
-      <c r="U24" s="124">
+      <c r="U24" s="125">
         <f>SUM(P24:T24)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="25" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D25" s="48"/>
-      <c r="E25" s="151"/>
+      <c r="E25" s="152"/>
       <c r="F25" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="147">
+      <c r="G25" s="148">
         <f>((G39+H39)/(1-L39))*$E$2</f>
         <v>432.1608040201005</v>
       </c>
-      <c r="H25" s="147"/>
+      <c r="H25" s="148"/>
       <c r="I25" s="87">
         <f>(I39/(1-L39))*$E$2</f>
         <v>331.65829145728645</v>
@@ -8998,14 +9012,14 @@
         <f>SUM(G25:K25)</f>
         <v>1000.0000000000001</v>
       </c>
-      <c r="N25" s="139"/>
+      <c r="N25" s="140"/>
       <c r="O25" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="142" t="s">
+      <c r="P25" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="Q25" s="142"/>
+      <c r="Q25" s="143"/>
       <c r="R25" s="84" t="s">
         <v>52</v>
       </c>
@@ -9025,11 +9039,11 @@
       <c r="F26" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="148">
+      <c r="G26" s="149">
         <f>G25/$L$7</f>
         <v>0.43216080402010049</v>
       </c>
-      <c r="H26" s="148"/>
+      <c r="H26" s="149"/>
       <c r="I26" s="112">
         <f t="shared" ref="I26" si="18">I25/$L$7</f>
         <v>0.33165829145728642</v>
@@ -9046,16 +9060,16 @@
         <f>SUM(G26:K26)</f>
         <v>1</v>
       </c>
-      <c r="N26" s="140"/>
-      <c r="O26" s="118" t="s">
+      <c r="N26" s="141"/>
+      <c r="O26" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="P26" s="143"/>
-      <c r="Q26" s="143"/>
-      <c r="R26" s="119"/>
-      <c r="S26" s="119"/>
-      <c r="T26" s="119"/>
-      <c r="U26" s="120"/>
+      <c r="P26" s="144"/>
+      <c r="Q26" s="144"/>
+      <c r="R26" s="120"/>
+      <c r="S26" s="120"/>
+      <c r="T26" s="120"/>
+      <c r="U26" s="121"/>
     </row>
     <row r="27" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D27" s="48"/>
@@ -9063,18 +9077,18 @@
       <c r="F27" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="152">
+      <c r="G27" s="153">
         <f>G23/G25</f>
         <v>0.34755813953488379</v>
       </c>
-      <c r="H27" s="152"/>
-      <c r="I27" s="123">
+      <c r="H27" s="153"/>
+      <c r="I27" s="124">
         <v>0.65</v>
       </c>
-      <c r="J27" s="123">
+      <c r="J27" s="124">
         <v>0.78</v>
       </c>
-      <c r="K27" s="123">
+      <c r="K27" s="124">
         <v>0.78</v>
       </c>
       <c r="L27" s="102"/>
@@ -9092,17 +9106,17 @@
     </row>
     <row r="29" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D29" s="97"/>
-      <c r="E29" s="150" t="s">
+      <c r="E29" s="151" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="153">
+      <c r="G29" s="154">
         <f>L29-K29-J29-I29</f>
         <v>180.18145161290317</v>
       </c>
-      <c r="H29" s="153"/>
+      <c r="H29" s="154"/>
       <c r="I29" s="82">
         <f>I33*I31</f>
         <v>203.125</v>
@@ -9122,10 +9136,10 @@
         <v>2</v>
       </c>
       <c r="O29" s="115"/>
-      <c r="P29" s="137" t="s">
+      <c r="P29" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="Q29" s="137"/>
+      <c r="Q29" s="138"/>
       <c r="R29" s="116" t="s">
         <v>6</v>
       </c>
@@ -9139,15 +9153,15 @@
     </row>
     <row r="30" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D30" s="97"/>
-      <c r="E30" s="151"/>
+      <c r="E30" s="152"/>
       <c r="F30" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="142">
+      <c r="G30" s="143">
         <f>G31-G29</f>
         <v>293.60887096774195</v>
       </c>
-      <c r="H30" s="142"/>
+      <c r="H30" s="143"/>
       <c r="I30" s="84">
         <f t="shared" ref="I30" si="22">I31-I29</f>
         <v>109.375</v>
@@ -9163,45 +9177,45 @@
       <c r="L30" s="99">
         <v>450</v>
       </c>
-      <c r="N30" s="138" t="s">
+      <c r="N30" s="139" t="s">
         <v>37</v>
       </c>
       <c r="O30" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P30" s="141">
+      <c r="P30" s="142">
         <f>(G31*G33/1000)/0.55</f>
         <v>0.32760263929618755</v>
       </c>
-      <c r="Q30" s="141"/>
-      <c r="R30" s="121">
+      <c r="Q30" s="142"/>
+      <c r="R30" s="122">
         <f>(I31*I33/1000)/0.55</f>
         <v>0.36931818181818177</v>
       </c>
-      <c r="S30" s="121">
+      <c r="S30" s="122">
         <f>(J31*J33/1000)/0.55</f>
         <v>0.27162756598240473</v>
       </c>
-      <c r="T30" s="121">
+      <c r="T30" s="122">
         <f>(K31*K33/1000)/0.55</f>
         <v>3.1451612903225887E-2</v>
       </c>
-      <c r="U30" s="124">
+      <c r="U30" s="125">
         <f>SUM(P30:T30)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D31" s="97"/>
-      <c r="E31" s="151"/>
+      <c r="E31" s="152"/>
       <c r="F31" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="147">
+      <c r="G31" s="148">
         <f>((G40+H40)/(1-L40))*$E$2</f>
         <v>473.79032258064512</v>
       </c>
-      <c r="H31" s="147"/>
+      <c r="H31" s="148"/>
       <c r="I31" s="87">
         <f>(I40/(1-L40))*$E$2</f>
         <v>312.5</v>
@@ -9218,14 +9232,14 @@
         <f>SUM(G31:K31)</f>
         <v>1000</v>
       </c>
-      <c r="N31" s="139"/>
+      <c r="N31" s="140"/>
       <c r="O31" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P31" s="142" t="s">
+      <c r="P31" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="Q31" s="142"/>
+      <c r="Q31" s="143"/>
       <c r="R31" s="84" t="s">
         <v>52</v>
       </c>
@@ -9245,11 +9259,11 @@
       <c r="F32" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="148">
+      <c r="G32" s="149">
         <f>G31/$L$7</f>
         <v>0.47379032258064513</v>
       </c>
-      <c r="H32" s="148"/>
+      <c r="H32" s="149"/>
       <c r="I32" s="112">
         <f t="shared" ref="I32" si="24">I31/$L$7</f>
         <v>0.3125</v>
@@ -9266,16 +9280,16 @@
         <f>SUM(G32:K32)</f>
         <v>1</v>
       </c>
-      <c r="N32" s="140"/>
-      <c r="O32" s="118" t="s">
+      <c r="N32" s="141"/>
+      <c r="O32" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="P32" s="143"/>
-      <c r="Q32" s="143"/>
-      <c r="R32" s="119"/>
-      <c r="S32" s="119"/>
-      <c r="T32" s="119"/>
-      <c r="U32" s="120"/>
+      <c r="P32" s="144"/>
+      <c r="Q32" s="144"/>
+      <c r="R32" s="120"/>
+      <c r="S32" s="120"/>
+      <c r="T32" s="120"/>
+      <c r="U32" s="121"/>
     </row>
     <row r="33" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="49"/>
@@ -9283,18 +9297,18 @@
       <c r="F33" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="149">
+      <c r="G33" s="150">
         <f>G29/G31</f>
         <v>0.38029787234042545</v>
       </c>
-      <c r="H33" s="149"/>
-      <c r="I33" s="123">
+      <c r="H33" s="150"/>
+      <c r="I33" s="124">
         <v>0.65</v>
       </c>
-      <c r="J33" s="123">
+      <c r="J33" s="124">
         <v>0.78</v>
       </c>
-      <c r="K33" s="123">
+      <c r="K33" s="124">
         <v>0.78</v>
       </c>
       <c r="L33" s="110"/>
@@ -9337,7 +9351,7 @@
       <c r="M35" s="27"/>
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D36" s="145" t="s">
+      <c r="D36" s="146" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="28" t="s">
@@ -9364,7 +9378,7 @@
       </c>
     </row>
     <row r="37" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D37" s="145"/>
+      <c r="D37" s="146"/>
       <c r="E37" s="28" t="s">
         <v>34</v>
       </c>
@@ -9389,7 +9403,7 @@
       </c>
     </row>
     <row r="38" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D38" s="145"/>
+      <c r="D38" s="146"/>
       <c r="E38" s="28" t="s">
         <v>35</v>
       </c>
@@ -9414,7 +9428,7 @@
       </c>
     </row>
     <row r="39" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D39" s="145"/>
+      <c r="D39" s="146"/>
       <c r="E39" s="28" t="s">
         <v>36</v>
       </c>
@@ -9439,7 +9453,7 @@
       </c>
     </row>
     <row r="40" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="146"/>
+      <c r="D40" s="147"/>
       <c r="E40" s="77" t="s">
         <v>37</v>
       </c>
@@ -9557,7 +9571,7 @@
   <dimension ref="B1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9566,9 +9580,10 @@
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -9580,15 +9595,21 @@
         <v>2</v>
       </c>
       <c r="D2" s="72"/>
-      <c r="E2" s="154" t="s">
+      <c r="E2" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="95" t="s">
+      <c r="F2" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="156" t="s">
+      <c r="G2" s="157" t="s">
         <v>118</v>
+      </c>
+      <c r="H2" s="132" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132" t="s">
+        <v>119</v>
       </c>
       <c r="R2" s="61" t="s">
         <v>31</v>
@@ -9601,20 +9622,31 @@
       <c r="B3" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="139" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="164">
-        <f>S8*H3/(1+S8)</f>
-        <v>435.41666666666669</v>
-      </c>
-      <c r="F3" s="164"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="170">
+      <c r="E3" s="166">
+        <f>E7*E5</f>
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F3" s="167">
+        <f>G3-E3</f>
+        <v>477.1</v>
+      </c>
+      <c r="G3" s="170">
         <v>550</v>
+      </c>
+      <c r="H3" s="183">
+        <f>(E3/F3)/(E4/F4)</f>
+        <v>3.8682059371862914</v>
+      </c>
+      <c r="I3" s="183"/>
+      <c r="J3" s="1">
+        <f>(E3/(E3+F3))/(E4/(E4+F4))</f>
+        <v>3.4880382775119632</v>
       </c>
       <c r="R3" s="61" t="s">
         <v>32</v>
@@ -9625,38 +9657,46 @@
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="97"/>
-      <c r="C4" s="145"/>
+      <c r="C4" s="140"/>
       <c r="D4" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="170">
+      <c r="E4" s="84">
+        <f>E5-E3</f>
+        <v>17.099999999999994</v>
+      </c>
+      <c r="F4" s="168">
+        <f>G4-E4</f>
+        <v>432.9</v>
+      </c>
+      <c r="G4" s="170">
         <v>450</v>
       </c>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
       <c r="R4" s="61"/>
       <c r="S4" s="60"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="48"/>
-      <c r="C5" s="145"/>
+      <c r="C5" s="140"/>
       <c r="D5" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="180">
-        <f>E6*H5</f>
+      <c r="E5" s="181">
+        <f>E6*G5</f>
         <v>90</v>
       </c>
-      <c r="F5" s="180"/>
-      <c r="G5" s="181">
-        <f>G6*H5</f>
+      <c r="F5" s="179">
+        <f>F6*G5</f>
         <v>910</v>
       </c>
-      <c r="H5" s="170">
-        <f>SUM(H3:H4)</f>
+      <c r="G5" s="170">
+        <f>SUM(G3:G4)</f>
         <v>1000</v>
       </c>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
       <c r="R5" s="61" t="s">
         <v>46</v>
       </c>
@@ -9664,7 +9704,7 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="48"/>
-      <c r="C6" s="97"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="113" t="s">
         <v>21</v>
       </c>
@@ -9672,12 +9712,13 @@
         <f>(0.5*E42)+(0.5*E50)</f>
         <v>0.09</v>
       </c>
-      <c r="F6" s="182"/>
-      <c r="G6" s="183">
+      <c r="F6" s="180">
         <f>1-E6</f>
         <v>0.91</v>
       </c>
-      <c r="H6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
       <c r="R6" s="27"/>
       <c r="S6" s="60" t="s">
         <v>26</v>
@@ -9685,14 +9726,20 @@
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="48"/>
-      <c r="C7" s="171"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="105"/>
+      <c r="E7" s="184">
+        <v>0.81</v>
+      </c>
+      <c r="F7" s="164">
+        <f>F3/F5</f>
+        <v>0.52428571428571435</v>
+      </c>
+      <c r="G7" s="105"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
       <c r="R7" s="27"/>
       <c r="S7" s="60"/>
     </row>
@@ -9702,8 +9749,9 @@
       <c r="D8" s="83"/>
       <c r="E8" s="103"/>
       <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
       <c r="R8" s="27" t="s">
         <v>116</v>
       </c>
@@ -9723,11 +9771,25 @@
       <c r="D9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="167"/>
-      <c r="H9" s="170">
+      <c r="E9" s="166">
+        <f>E13*E11</f>
+        <v>92</v>
+      </c>
+      <c r="F9" s="167">
+        <f>G9-E9</f>
+        <v>458</v>
+      </c>
+      <c r="G9" s="170">
         <v>550</v>
+      </c>
+      <c r="H9" s="183">
+        <f>(E9/F9)/(E10/F10)</f>
+        <v>3.7292576419213996</v>
+      </c>
+      <c r="I9" s="183"/>
+      <c r="J9" s="1">
+        <f>(E9/(E9+F9))/(E10/(E10+F10))</f>
+        <v>3.2727272727272747</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
@@ -9736,16 +9798,23 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="97"/>
-      <c r="C10" s="145"/>
+      <c r="C10" s="146"/>
       <c r="D10" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="170">
+      <c r="E10" s="84">
+        <f>E11-E9</f>
+        <v>22.999999999999986</v>
+      </c>
+      <c r="F10" s="168">
+        <f>G10-E10</f>
+        <v>427</v>
+      </c>
+      <c r="G10" s="170">
         <v>450</v>
       </c>
+      <c r="H10" s="183"/>
+      <c r="I10" s="183"/>
       <c r="R10" s="27"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -9753,23 +9822,24 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="97"/>
-      <c r="C11" s="145"/>
+      <c r="C11" s="146"/>
       <c r="D11" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="165">
-        <f>E12*H11</f>
+      <c r="E11" s="162">
+        <f>E12*G11</f>
         <v>114.99999999999999</v>
       </c>
-      <c r="F11" s="165"/>
-      <c r="G11" s="166">
-        <f>G12*H11</f>
+      <c r="F11" s="165">
+        <f>F12*G11</f>
         <v>885</v>
       </c>
-      <c r="H11" s="170">
-        <f>SUM(H9:H10)</f>
+      <c r="G11" s="170">
+        <f>SUM(G9:G10)</f>
         <v>1000</v>
       </c>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="97"/>
@@ -9781,12 +9851,13 @@
         <f>(0.5*E43)+(0.5*E51)</f>
         <v>0.11499999999999999</v>
       </c>
-      <c r="F12" s="161"/>
-      <c r="G12" s="162">
+      <c r="F12" s="163">
         <f>1-E12</f>
         <v>0.88500000000000001</v>
       </c>
-      <c r="H12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="183"/>
+      <c r="I12" s="183"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="97"/>
@@ -9794,10 +9865,16 @@
       <c r="D13" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="105"/>
+      <c r="E13" s="184">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="164">
+        <f>F9/F11</f>
+        <v>0.51751412429378529</v>
+      </c>
+      <c r="G13" s="105"/>
+      <c r="H13" s="183"/>
+      <c r="I13" s="183"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="97"/>
@@ -9805,8 +9882,9 @@
       <c r="D14" s="83"/>
       <c r="E14" s="84"/>
       <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="183"/>
+      <c r="I14" s="183"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="97"/>
@@ -9816,47 +9894,69 @@
       <c r="D15" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="164"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="170">
+      <c r="E15" s="166">
+        <f>E19*E17</f>
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F15" s="167">
+        <f>G15-E15</f>
+        <v>477.1</v>
+      </c>
+      <c r="G15" s="170">
         <v>550</v>
+      </c>
+      <c r="H15" s="183">
+        <f>(E15/F15)/(E16/F16)</f>
+        <v>3.8682059371862914</v>
+      </c>
+      <c r="I15" s="183"/>
+      <c r="J15" s="1">
+        <f>(E15/(E15+F15))/(E16/(E16+F16))</f>
+        <v>3.4880382775119632</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="48"/>
-      <c r="C16" s="145"/>
+      <c r="C16" s="146"/>
       <c r="D16" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="168"/>
-      <c r="H16" s="170">
+      <c r="E16" s="84">
+        <f>E17-E15</f>
+        <v>17.099999999999994</v>
+      </c>
+      <c r="F16" s="168">
+        <f>G16-E16</f>
+        <v>432.9</v>
+      </c>
+      <c r="G16" s="170">
         <v>450</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="183"/>
+      <c r="I16" s="183"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="48"/>
-      <c r="C17" s="145"/>
+      <c r="C17" s="146"/>
       <c r="D17" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="165">
-        <f>E18*H17</f>
+      <c r="E17" s="162">
+        <f>E18*G17</f>
         <v>90</v>
       </c>
-      <c r="F17" s="165"/>
-      <c r="G17" s="166">
-        <f>G18*H17</f>
+      <c r="F17" s="165">
+        <f>F18*G17</f>
         <v>910</v>
       </c>
-      <c r="H17" s="170">
-        <f>SUM(H15:H16)</f>
+      <c r="G17" s="170">
+        <f>SUM(G15:G16)</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="183"/>
+      <c r="I17" s="183"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="48"/>
       <c r="C18" s="46"/>
       <c r="D18" s="113" t="s">
@@ -9866,34 +9966,42 @@
         <f>(0.5*E44)+(0.5*E52)</f>
         <v>0.09</v>
       </c>
-      <c r="F18" s="161"/>
-      <c r="G18" s="162">
+      <c r="F18" s="163">
         <f>1-E18</f>
         <v>0.91</v>
       </c>
-      <c r="H18" s="105"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="105"/>
+      <c r="H18" s="183"/>
+      <c r="I18" s="183"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="48"/>
       <c r="C19" s="172"/>
       <c r="D19" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="160"/>
-      <c r="F19" s="160"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="105"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="184">
+        <v>0.81</v>
+      </c>
+      <c r="F19" s="164">
+        <f>F15/F17</f>
+        <v>0.52428571428571435</v>
+      </c>
+      <c r="G19" s="105"/>
+      <c r="H19" s="183"/>
+      <c r="I19" s="183"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="48"/>
       <c r="C20" s="46"/>
       <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="105"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="48"/>
       <c r="C21" s="173" t="s">
         <v>34</v>
@@ -9901,47 +10009,69 @@
       <c r="D21" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="164"/>
-      <c r="F21" s="164"/>
-      <c r="G21" s="167"/>
-      <c r="H21" s="170">
+      <c r="E21" s="166">
+        <f>E25*E23</f>
+        <v>112</v>
+      </c>
+      <c r="F21" s="167">
+        <f>G21-E21</f>
+        <v>438</v>
+      </c>
+      <c r="G21" s="170">
         <v>550</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="183">
+        <f>(E21/F21)/(E22/F22)</f>
+        <v>3.8538812785388123</v>
+      </c>
+      <c r="I21" s="183"/>
+      <c r="J21" s="1">
+        <f>(E21/(E21+F21))/(E22/(E22+F22))</f>
+        <v>3.2727272727272729</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="48"/>
       <c r="C22" s="174"/>
       <c r="D22" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="142"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="168"/>
-      <c r="H22" s="170">
+      <c r="E22" s="84">
+        <f>E23-E21</f>
+        <v>28</v>
+      </c>
+      <c r="F22" s="168">
+        <f>G22-E22</f>
+        <v>422</v>
+      </c>
+      <c r="G22" s="170">
         <v>450</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="183"/>
+      <c r="I22" s="183"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="48"/>
       <c r="C23" s="174"/>
       <c r="D23" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="165">
-        <f>E24*H23</f>
+      <c r="E23" s="162">
+        <f>E24*G23</f>
         <v>140</v>
       </c>
-      <c r="F23" s="165"/>
-      <c r="G23" s="166">
-        <f>G24*H23</f>
+      <c r="F23" s="165">
+        <f>F24*G23</f>
         <v>860</v>
       </c>
-      <c r="H23" s="170">
-        <f>SUM(H21:H22)</f>
+      <c r="G23" s="170">
+        <f>SUM(G21:G22)</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="183"/>
+      <c r="I23" s="183"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="48"/>
       <c r="C24" s="46"/>
       <c r="D24" s="113" t="s">
@@ -9951,34 +10081,42 @@
         <f>(0.5*E45)+(0.5*E53)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="F24" s="161"/>
-      <c r="G24" s="162">
+      <c r="F24" s="163">
         <f>1-E24</f>
         <v>0.86</v>
       </c>
-      <c r="H24" s="105"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="105"/>
+      <c r="H24" s="183"/>
+      <c r="I24" s="183"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="48"/>
       <c r="C25" s="172"/>
       <c r="D25" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="160"/>
-      <c r="F25" s="160"/>
-      <c r="G25" s="163"/>
-      <c r="H25" s="105"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="184">
+        <v>0.8</v>
+      </c>
+      <c r="F25" s="164">
+        <f>F21/F23</f>
+        <v>0.50930232558139532</v>
+      </c>
+      <c r="G25" s="105"/>
+      <c r="H25" s="183"/>
+      <c r="I25" s="183"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="97"/>
       <c r="C26" s="97"/>
       <c r="D26" s="35"/>
       <c r="E26" s="83"/>
       <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="105"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="105"/>
+      <c r="H26" s="183"/>
+      <c r="I26" s="183"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="97"/>
       <c r="C27" s="173" t="s">
         <v>35</v>
@@ -9986,47 +10124,69 @@
       <c r="D27" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="164"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="167"/>
-      <c r="H27" s="170">
+      <c r="E27" s="166">
+        <f>E31*E29</f>
+        <v>142.20000000000002</v>
+      </c>
+      <c r="F27" s="167">
+        <f>G27-E27</f>
+        <v>407.79999999999995</v>
+      </c>
+      <c r="G27" s="170">
         <v>550</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="183">
+        <f>(E27/F27)/(E28/F28)</f>
+        <v>3.8024942198556744</v>
+      </c>
+      <c r="I27" s="183"/>
+      <c r="J27" s="1">
+        <f>(E27/(E27+F27))/(E28/(E28+F28))</f>
+        <v>3.0779220779220795</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="97"/>
       <c r="C28" s="174"/>
       <c r="D28" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="168"/>
-      <c r="H28" s="170">
+      <c r="E28" s="84">
+        <f>E29-E27</f>
+        <v>37.799999999999983</v>
+      </c>
+      <c r="F28" s="168">
+        <f>G28-E28</f>
+        <v>412.20000000000005</v>
+      </c>
+      <c r="G28" s="170">
         <v>450</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="183"/>
+      <c r="I28" s="183"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="97"/>
       <c r="C29" s="174"/>
       <c r="D29" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="165">
-        <f>E30*H29</f>
+      <c r="E29" s="162">
+        <f>E30*G29</f>
         <v>180</v>
       </c>
-      <c r="F29" s="165"/>
-      <c r="G29" s="166">
-        <f>G30*H29</f>
+      <c r="F29" s="165">
+        <f>F30*G29</f>
         <v>820.00000000000011</v>
       </c>
-      <c r="H29" s="170">
-        <f>SUM(H27:H28)</f>
+      <c r="G29" s="170">
+        <f>SUM(G27:G28)</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="183"/>
+      <c r="I29" s="183"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="97"/>
       <c r="C30" s="46"/>
       <c r="D30" s="113" t="s">
@@ -10036,34 +10196,42 @@
         <f>(0.5*E46)+(0.5*E54)</f>
         <v>0.18</v>
       </c>
-      <c r="F30" s="161"/>
-      <c r="G30" s="162">
+      <c r="F30" s="163">
         <f>1-E30</f>
         <v>0.82000000000000006</v>
       </c>
-      <c r="H30" s="105"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="105"/>
+      <c r="H30" s="183"/>
+      <c r="I30" s="183"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="97"/>
       <c r="C31" s="172"/>
       <c r="D31" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="105"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="184">
+        <v>0.79</v>
+      </c>
+      <c r="F31" s="164">
+        <f>F27/F29</f>
+        <v>0.49731707317073159</v>
+      </c>
+      <c r="G31" s="105"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="183"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="97"/>
       <c r="C32" s="97"/>
       <c r="D32" s="35"/>
       <c r="E32" s="83"/>
       <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="105"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="105"/>
+      <c r="H32" s="183"/>
+      <c r="I32" s="183"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="97"/>
       <c r="C33" s="173" t="s">
         <v>101</v>
@@ -10071,47 +10239,69 @@
       <c r="D33" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="164"/>
-      <c r="F33" s="164"/>
-      <c r="G33" s="167"/>
-      <c r="H33" s="170">
+      <c r="E33" s="166">
+        <f>E37*E35</f>
+        <v>183.30000000000004</v>
+      </c>
+      <c r="F33" s="167">
+        <f>G33-E33</f>
+        <v>366.69999999999993</v>
+      </c>
+      <c r="G33" s="170">
         <v>550</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="183">
+        <f>(E33/F33)/(E34/F34)</f>
+        <v>3.8509804893770014</v>
+      </c>
+      <c r="I33" s="183"/>
+      <c r="J33" s="1">
+        <f>(E33/(E33+F33))/(E34/(E34+F34))</f>
+        <v>2.900826446280993</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="97"/>
       <c r="C34" s="174"/>
       <c r="D34" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="168"/>
-      <c r="H34" s="170">
+      <c r="E34" s="84">
+        <f>E35-E33</f>
+        <v>51.699999999999989</v>
+      </c>
+      <c r="F34" s="168">
+        <f>G34-E34</f>
+        <v>398.3</v>
+      </c>
+      <c r="G34" s="170">
         <v>450</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="183"/>
+      <c r="I34" s="183"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="97"/>
       <c r="C35" s="174"/>
       <c r="D35" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="165">
-        <f>E36*H35</f>
+      <c r="E35" s="162">
+        <f>E36*G35</f>
         <v>235.00000000000003</v>
       </c>
-      <c r="F35" s="165"/>
-      <c r="G35" s="166">
-        <f>G36*H35</f>
+      <c r="F35" s="165">
+        <f>F36*G35</f>
         <v>765</v>
       </c>
-      <c r="H35" s="170">
-        <f>SUM(H33:H34)</f>
+      <c r="G35" s="170">
+        <f>SUM(G33:G34)</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="97"/>
       <c r="C36" s="46"/>
       <c r="D36" s="113" t="s">
@@ -10121,27 +10311,36 @@
         <f>(0.5*E47)+(0.5*E55)</f>
         <v>0.23500000000000001</v>
       </c>
-      <c r="F36" s="161"/>
-      <c r="G36" s="162">
+      <c r="F36" s="163">
         <f>1-E36</f>
         <v>0.76500000000000001</v>
       </c>
-      <c r="H36" s="105"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="105"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="49"/>
       <c r="C37" s="176"/>
       <c r="D37" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="178"/>
-      <c r="F37" s="178"/>
-      <c r="G37" s="179"/>
-      <c r="H37" s="175"/>
-    </row>
-    <row r="38" spans="2:8" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="185">
+        <v>0.78</v>
+      </c>
+      <c r="F37" s="178">
+        <f>F33/F35</f>
+        <v>0.4793464052287581</v>
+      </c>
+      <c r="G37" s="175"/>
+      <c r="H37" s="183"/>
+      <c r="I37" s="183"/>
+    </row>
+    <row r="38" spans="2:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="28"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="111" t="s">
         <v>48</v>
       </c>
@@ -10152,12 +10351,12 @@
       <c r="E41" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="156" t="s">
+      <c r="F41" s="157" t="s">
         <v>102</v>
       </c>
       <c r="G41" s="28"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
         <v>99</v>
       </c>
@@ -10165,93 +10364,90 @@
         <v>97</v>
       </c>
       <c r="D42" s="35"/>
-      <c r="E42" s="155">
+      <c r="E42" s="156">
         <v>0.08</v>
       </c>
-      <c r="F42" s="157" t="s">
+      <c r="F42" s="158" t="s">
         <v>109</v>
       </c>
       <c r="G42" s="28"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="145" t="s">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="146" t="s">
         <v>95</v>
       </c>
       <c r="C43" s="28" t="s">
         <v>98</v>
       </c>
       <c r="D43" s="35"/>
-      <c r="E43" s="155">
+      <c r="E43" s="156">
         <v>0.12</v>
       </c>
-      <c r="F43" s="157" t="s">
+      <c r="F43" s="158" t="s">
         <v>105</v>
       </c>
       <c r="G43" s="28"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="145"/>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="146"/>
       <c r="C44" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D44" s="35"/>
-      <c r="E44" s="155">
+      <c r="E44" s="156">
         <v>0.12</v>
       </c>
-      <c r="F44" s="157" t="s">
+      <c r="F44" s="158" t="s">
         <v>106</v>
       </c>
       <c r="G44" s="28"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="145"/>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="146"/>
       <c r="C45" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D45" s="35"/>
-      <c r="E45" s="155">
+      <c r="E45" s="156">
         <v>0.16</v>
       </c>
-      <c r="F45" s="157" t="s">
+      <c r="F45" s="158" t="s">
         <v>104</v>
       </c>
       <c r="G45" s="28"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="145"/>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="146"/>
       <c r="C46" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D46" s="35"/>
-      <c r="E46" s="155">
+      <c r="E46" s="156">
         <v>0.18</v>
       </c>
-      <c r="F46" s="157" t="s">
+      <c r="F46" s="158" t="s">
         <v>107</v>
       </c>
       <c r="G46" s="28"/>
     </row>
-    <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="146"/>
+    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="147"/>
       <c r="C47" s="77" t="s">
         <v>101</v>
       </c>
       <c r="D47" s="78"/>
-      <c r="E47" s="158">
+      <c r="E47" s="159">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F47" s="159" t="s">
+      <c r="F47" s="160" t="s">
         <v>108</v>
       </c>
       <c r="G47" s="28"/>
     </row>
-    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="111" t="s">
@@ -10264,7 +10460,7 @@
       <c r="E49" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="156" t="s">
+      <c r="F49" s="157" t="s">
         <v>102</v>
       </c>
       <c r="G49" s="28"/>
@@ -10277,127 +10473,96 @@
         <v>97</v>
       </c>
       <c r="D50" s="35"/>
-      <c r="E50" s="155">
+      <c r="E50" s="156">
         <v>0.1</v>
       </c>
-      <c r="F50" s="157" t="s">
+      <c r="F50" s="158" t="s">
         <v>110</v>
       </c>
       <c r="G50" s="28"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="145" t="s">
+      <c r="B51" s="146" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>98</v>
       </c>
       <c r="D51" s="35"/>
-      <c r="E51" s="155">
+      <c r="E51" s="156">
         <v>0.11</v>
       </c>
-      <c r="F51" s="157" t="s">
+      <c r="F51" s="158" t="s">
         <v>111</v>
       </c>
       <c r="G51" s="28"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="145"/>
+      <c r="B52" s="146"/>
       <c r="C52" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="35"/>
-      <c r="E52" s="155">
+      <c r="E52" s="156">
         <v>0.06</v>
       </c>
-      <c r="F52" s="157" t="s">
+      <c r="F52" s="158" t="s">
         <v>112</v>
       </c>
       <c r="G52" s="28"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="145"/>
+      <c r="B53" s="146"/>
       <c r="C53" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="35"/>
-      <c r="E53" s="155">
+      <c r="E53" s="156">
         <v>0.12</v>
       </c>
-      <c r="F53" s="157" t="s">
+      <c r="F53" s="158" t="s">
         <v>103</v>
       </c>
       <c r="G53" s="28"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="145"/>
+      <c r="B54" s="146"/>
       <c r="C54" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D54" s="35"/>
-      <c r="E54" s="155">
+      <c r="E54" s="156">
         <v>0.18</v>
       </c>
-      <c r="F54" s="157" t="s">
+      <c r="F54" s="158" t="s">
         <v>107</v>
       </c>
       <c r="G54" s="28"/>
     </row>
     <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="146"/>
+      <c r="B55" s="147"/>
       <c r="C55" s="77" t="s">
         <v>101</v>
       </c>
       <c r="D55" s="78"/>
-      <c r="E55" s="158">
+      <c r="E55" s="159">
         <v>0.19</v>
       </c>
-      <c r="F55" s="159" t="s">
+      <c r="F55" s="160" t="s">
         <v>113</v>
       </c>
       <c r="G55" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="E33:F33"/>
+  <mergeCells count="8">
     <mergeCell ref="B51:B55"/>
     <mergeCell ref="B43:B47"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10438,43 +10603,43 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="127" t="s">
+      <c r="E3" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="127" t="s">
+      <c r="F3" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="G3" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="127" t="s">
+      <c r="H3" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="127" t="s">
+      <c r="M3" s="128" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="127" t="s">
+      <c r="N3" s="128" t="s">
         <v>85</v>
       </c>
     </row>
@@ -10491,13 +10656,13 @@
       <c r="E4" s="1">
         <v>0.6</v>
       </c>
-      <c r="F4" s="129" t="s">
+      <c r="F4" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="130" t="s">
+      <c r="G4" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="129" t="s">
+      <c r="H4" s="130" t="s">
         <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -10532,10 +10697,10 @@
       <c r="E5" s="1">
         <v>0.6</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="F5" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="130" t="s">
+      <c r="G5" s="131" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -10573,10 +10738,10 @@
       <c r="E6" s="1">
         <v>0.6</v>
       </c>
-      <c r="F6" s="129" t="s">
+      <c r="F6" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="130" t="s">
+      <c r="G6" s="131" t="s">
         <v>83</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -10614,10 +10779,10 @@
       <c r="E7" s="1">
         <v>0.6</v>
       </c>
-      <c r="F7" s="129" t="s">
+      <c r="F7" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="130" t="s">
+      <c r="G7" s="131" t="s">
         <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -10658,56 +10823,56 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:20" s="126" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="127" t="s">
+    <row r="10" spans="2:20" s="127" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="127" t="s">
+      <c r="C10" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="127" t="s">
+      <c r="E10" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="127" t="s">
+      <c r="F10" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="127" t="s">
+      <c r="G10" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="127" t="s">
+      <c r="H10" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="127" t="s">
+      <c r="I10" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="127" t="s">
+      <c r="J10" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="127" t="s">
+      <c r="K10" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="127" t="s">
+      <c r="L10" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="127" t="s">
+      <c r="M10" s="128" t="s">
         <v>86</v>
       </c>
-      <c r="N10" s="127" t="s">
+      <c r="N10" s="128" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="126" t="s">
+      <c r="Q10" s="127" t="s">
         <v>63</v>
       </c>
-      <c r="R10" s="128">
+      <c r="R10" s="129">
         <v>1</v>
       </c>
-      <c r="S10" s="125" t="s">
+      <c r="S10" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="T10" s="125" t="s">
+      <c r="T10" s="126" t="s">
         <v>65</v>
       </c>
     </row>
@@ -10724,13 +10889,13 @@
       <c r="E11" s="1">
         <v>0.6</v>
       </c>
-      <c r="F11" s="129" t="s">
+      <c r="F11" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="130" t="s">
+      <c r="G11" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="129" t="s">
+      <c r="H11" s="130" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -10774,10 +10939,10 @@
       <c r="E12" s="1">
         <v>0.6</v>
       </c>
-      <c r="F12" s="129" t="s">
+      <c r="F12" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="129" t="s">
+      <c r="G12" s="130" t="s">
         <v>84</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -10824,10 +10989,10 @@
       <c r="E13" s="1">
         <v>0.6</v>
       </c>
-      <c r="F13" s="129" t="s">
+      <c r="F13" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="129" t="s">
+      <c r="G13" s="130" t="s">
         <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -10865,10 +11030,10 @@
       <c r="E14" s="1">
         <v>0.6</v>
       </c>
-      <c r="F14" s="129" t="s">
+      <c r="F14" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="129" t="s">
+      <c r="G14" s="130" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="1" t="s">

</xml_diff>

<commit_message>
updated atrophy reference, HP prevalence reference
</commit_message>
<xml_diff>
--- a/docs/source/concept_models/vivarium_swissre_stomachcancer/precancer_states_and_hpylori_memo_28dec2020.xlsx
+++ b/docs/source/concept_models/vivarium_swissre_stomachcancer/precancer_states_and_hpylori_memo_28dec2020.xlsx
@@ -9,15 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="19155" windowHeight="6330" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="17355" windowHeight="10920" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="You 1993" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
-    <sheet name="Kang 2015" sheetId="5" r:id="rId3"/>
-    <sheet name="H pylori by state" sheetId="2" r:id="rId4"/>
-    <sheet name="Aoki 2005" sheetId="7" r:id="rId5"/>
-    <sheet name="sample simulant" sheetId="4" r:id="rId6"/>
+    <sheet name="Kang 2015" sheetId="5" r:id="rId2"/>
+    <sheet name="H pylori by state" sheetId="2" r:id="rId3"/>
+    <sheet name="Wang 2020" sheetId="7" r:id="rId4"/>
+    <sheet name="sample simulant" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="117">
   <si>
     <t>Male</t>
   </si>
@@ -316,63 +315,9 @@
     <t>NCG</t>
   </si>
   <si>
-    <t>Aoki 2005, fig 5</t>
-  </si>
-  <si>
-    <t>Aoki 2005, fig 6</t>
-  </si>
-  <si>
-    <t>&lt;30</t>
-  </si>
-  <si>
-    <t>30-39</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>70+</t>
-  </si>
-  <si>
     <t xml:space="preserve">95%CI </t>
   </si>
   <si>
-    <t>0.08-0.16</t>
-  </si>
-  <si>
-    <t>0.08-0.24</t>
-  </si>
-  <si>
-    <t>0.06-0.18</t>
-  </si>
-  <si>
-    <t>0.07-0.17</t>
-  </si>
-  <si>
-    <t>0.10-0.26</t>
-  </si>
-  <si>
-    <t>0.06-0.50</t>
-  </si>
-  <si>
-    <t>0.00-0.18</t>
-  </si>
-  <si>
-    <t>0.00-0.20</t>
-  </si>
-  <si>
-    <t>0.09-0.13</t>
-  </si>
-  <si>
-    <t>0.04-0.08</t>
-  </si>
-  <si>
-    <t>0.08-0.30</t>
-  </si>
-  <si>
     <t>atrophy +</t>
   </si>
   <si>
@@ -395,18 +340,58 @@
   </si>
   <si>
     <t>p_atrophy</t>
+  </si>
+  <si>
+    <t>per 1000</t>
+  </si>
+  <si>
+    <t>Gastritis %</t>
+  </si>
+  <si>
+    <t>MALE &amp; FEMALE</t>
+  </si>
+  <si>
+    <t>&lt;20</t>
+  </si>
+  <si>
+    <t>20-39</t>
+  </si>
+  <si>
+    <t>0.22-0.79</t>
+  </si>
+  <si>
+    <t>Wang 2020</t>
+  </si>
+  <si>
+    <t>40-59</t>
+  </si>
+  <si>
+    <t>1.14-1.76</t>
+  </si>
+  <si>
+    <t>60-79</t>
+  </si>
+  <si>
+    <t>3.01-5.25</t>
+  </si>
+  <si>
+    <t>&gt;=80</t>
+  </si>
+  <si>
+    <t>0.67-18.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -886,7 +871,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,9 +1141,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1221,115 +1203,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1348,9 +1287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1372,9 +1308,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1383,12 +1316,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1406,16 +1333,95 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2121,7 +2127,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2695,7 +2700,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4170,7 +4174,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6605,44 +6608,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>318457</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>1707</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7255669" y="7243762"/>
-          <a:ext cx="5028569" cy="5402383"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>25</xdr:row>
@@ -6652,7 +6617,7 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>149445</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>173175</xdr:rowOff>
+      <xdr:rowOff>185081</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6662,7 +6627,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6970,12 +6935,12 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -7774,18 +7739,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K9"/>
   <sheetViews>
@@ -8008,7 +7961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AC44"/>
   <sheetViews>
@@ -8054,16 +8007,16 @@
       <c r="E2" s="59">
         <v>1000</v>
       </c>
-      <c r="N2" s="137" t="s">
+      <c r="N2" s="182" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="137"/>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="137"/>
-      <c r="S2" s="137"/>
-      <c r="T2" s="137"/>
-      <c r="U2" s="137"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182"/>
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="61" t="s">
@@ -8084,10 +8037,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="72"/>
-      <c r="G4" s="155" t="s">
+      <c r="G4" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="155"/>
+      <c r="H4" s="165"/>
       <c r="I4" s="94" t="s">
         <v>6</v>
       </c>
@@ -8097,27 +8050,27 @@
       <c r="K4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="96" t="s">
+      <c r="L4" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="114" t="s">
+      <c r="N4" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="115"/>
-      <c r="P4" s="138" t="s">
+      <c r="O4" s="114"/>
+      <c r="P4" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="116" t="s">
+      <c r="Q4" s="177"/>
+      <c r="R4" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="116" t="s">
+      <c r="S4" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="116" t="s">
+      <c r="T4" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="117"/>
+      <c r="U4" s="116"/>
       <c r="W4" s="44"/>
       <c r="X4" s="62"/>
       <c r="Y4" s="67" t="s">
@@ -8132,7 +8085,7 @@
       <c r="AB4" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="134"/>
+      <c r="AC4" s="132"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
@@ -8141,20 +8094,20 @@
       <c r="B5" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="139" t="s">
+      <c r="E5" s="170" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="154">
+      <c r="G5" s="166">
         <f>L5-K5-J5-I5</f>
         <v>309.5</v>
       </c>
-      <c r="H5" s="154"/>
+      <c r="H5" s="166"/>
       <c r="I5" s="82">
         <f>I9*I7</f>
         <v>162.5</v>
@@ -8167,50 +8120,50 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="98">
+      <c r="L5" s="97">
         <v>550</v>
       </c>
-      <c r="N5" s="139" t="s">
+      <c r="N5" s="170" t="s">
         <v>33</v>
       </c>
       <c r="O5" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="145">
+      <c r="P5" s="179">
         <f>(G7*G9/1000)/0.55</f>
         <v>0.56272727272727263</v>
       </c>
-      <c r="Q5" s="145"/>
-      <c r="R5" s="123">
+      <c r="Q5" s="179"/>
+      <c r="R5" s="121">
         <f>(I7*I9/1000)/0.55</f>
         <v>0.29545454545454541</v>
       </c>
-      <c r="S5" s="123">
+      <c r="S5" s="121">
         <f>(J7*J9/1000)/0.55</f>
         <v>0.14181818181818182</v>
       </c>
-      <c r="T5" s="123">
+      <c r="T5" s="121">
         <f>(K7*K9/1000)/0.55</f>
         <v>0</v>
       </c>
-      <c r="U5" s="125">
+      <c r="U5" s="123">
         <f>SUM(P5:T5)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="W5" s="132" t="s">
+      <c r="W5" s="130" t="s">
         <v>33</v>
       </c>
       <c r="X5" s="81"/>
-      <c r="Y5" s="135">
+      <c r="Y5" s="133">
         <v>0.42699999999999999</v>
       </c>
-      <c r="Z5" s="135">
+      <c r="Z5" s="133">
         <v>0.45864045864045866</v>
       </c>
-      <c r="AA5" s="135">
+      <c r="AA5" s="133">
         <v>0.2424242424242424</v>
       </c>
-      <c r="AB5" s="135">
+      <c r="AB5" s="133">
         <v>1.6380016380015937E-3</v>
       </c>
       <c r="AC5" s="75"/>
@@ -8220,16 +8173,16 @@
       <c r="B6" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="97"/>
-      <c r="E6" s="140"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="171"/>
       <c r="F6" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="143">
+      <c r="G6" s="167">
         <f>G7-G5</f>
         <v>340.5</v>
       </c>
-      <c r="H6" s="143"/>
+      <c r="H6" s="167"/>
       <c r="I6" s="84">
         <f t="shared" ref="I6:J6" si="1">I7-I5</f>
         <v>87.5</v>
@@ -8242,17 +8195,17 @@
         <f>K7-K5</f>
         <v>0</v>
       </c>
-      <c r="L6" s="99">
+      <c r="L6" s="98">
         <v>450</v>
       </c>
-      <c r="N6" s="140"/>
+      <c r="N6" s="171"/>
       <c r="O6" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="143" t="s">
+      <c r="P6" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="143"/>
+      <c r="Q6" s="167"/>
       <c r="R6" s="84" t="s">
         <v>52</v>
       </c>
@@ -8287,15 +8240,15 @@
         <v>27</v>
       </c>
       <c r="D7" s="48"/>
-      <c r="E7" s="140"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="148">
+      <c r="G7" s="168">
         <f>((G36+H36)/(1-L36))*$E$2</f>
         <v>650</v>
       </c>
-      <c r="H7" s="148"/>
+      <c r="H7" s="168"/>
       <c r="I7" s="87">
         <f>(I36/(1-L36))*$E$2</f>
         <v>250</v>
@@ -8308,21 +8261,21 @@
         <f>(K36/(1-N36))*$E$2</f>
         <v>0</v>
       </c>
-      <c r="L7" s="100">
+      <c r="L7" s="99">
         <f>SUM(G7:K7)</f>
         <v>1000</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="119" t="s">
+      <c r="N7" s="178"/>
+      <c r="O7" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="144"/>
-      <c r="Q7" s="144"/>
-      <c r="R7" s="120"/>
-      <c r="S7" s="120"/>
-      <c r="T7" s="120"/>
-      <c r="U7" s="121"/>
-      <c r="W7" s="133" t="s">
+      <c r="P7" s="174"/>
+      <c r="Q7" s="174"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="118"/>
+      <c r="T7" s="118"/>
+      <c r="U7" s="119"/>
+      <c r="W7" s="131" t="s">
         <v>92</v>
       </c>
       <c r="Y7" s="58">
@@ -8345,27 +8298,27 @@
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="91"/>
-      <c r="F8" s="113" t="s">
+      <c r="F8" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="149">
+      <c r="G8" s="169">
         <f>G7/$L$7</f>
         <v>0.65</v>
       </c>
-      <c r="H8" s="149"/>
-      <c r="I8" s="112">
+      <c r="H8" s="169"/>
+      <c r="I8" s="111">
         <f t="shared" ref="I8:L8" si="2">I7/$L$7</f>
         <v>0.25</v>
       </c>
-      <c r="J8" s="112">
+      <c r="J8" s="111">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K8" s="112">
+      <c r="K8" s="111">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8" s="101">
+      <c r="L8" s="100">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -8395,21 +8348,21 @@
       <c r="F9" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="153">
+      <c r="G9" s="164">
         <f>G5/G7</f>
         <v>0.47615384615384615</v>
       </c>
-      <c r="H9" s="153"/>
-      <c r="I9" s="124">
+      <c r="H9" s="164"/>
+      <c r="I9" s="122">
         <v>0.65</v>
       </c>
-      <c r="J9" s="124">
+      <c r="J9" s="122">
         <v>0.78</v>
       </c>
-      <c r="K9" s="124">
+      <c r="K9" s="122">
         <v>0.78</v>
       </c>
-      <c r="L9" s="102"/>
+      <c r="L9" s="101"/>
       <c r="W9" s="1" t="s">
         <v>37</v>
       </c>
@@ -8430,27 +8383,27 @@
       <c r="D10" s="48"/>
       <c r="E10" s="83"/>
       <c r="F10" s="83"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="105"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="104"/>
       <c r="Y10" s="27"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D11" s="97"/>
-      <c r="E11" s="139" t="s">
+      <c r="D11" s="96"/>
+      <c r="E11" s="170" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="154">
+      <c r="G11" s="166">
         <f>L11-K11-J11-I11</f>
         <v>251.48148148148147</v>
       </c>
-      <c r="H11" s="154"/>
+      <c r="H11" s="166"/>
       <c r="I11" s="82">
         <f>I15*I13</f>
         <v>182.1821821821822</v>
@@ -8463,40 +8416,40 @@
         <f t="shared" si="3"/>
         <v>0.78078078078075974</v>
       </c>
-      <c r="L11" s="98">
+      <c r="L11" s="97">
         <v>550</v>
       </c>
-      <c r="N11" s="114" t="s">
+      <c r="N11" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="115"/>
-      <c r="P11" s="138" t="s">
+      <c r="O11" s="114"/>
+      <c r="P11" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" s="138"/>
-      <c r="R11" s="116" t="s">
+      <c r="Q11" s="177"/>
+      <c r="R11" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="S11" s="116" t="s">
+      <c r="S11" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="T11" s="116" t="s">
+      <c r="T11" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="U11" s="117"/>
+      <c r="U11" s="116"/>
       <c r="Y11" s="27"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D12" s="97"/>
-      <c r="E12" s="140"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="171"/>
       <c r="F12" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="143">
+      <c r="G12" s="167">
         <f>G13-G11</f>
         <v>319.08908908908899</v>
       </c>
-      <c r="H12" s="143"/>
+      <c r="H12" s="167"/>
       <c r="I12" s="84">
         <f t="shared" ref="I12" si="4">I13-I11</f>
         <v>98.098098098098092</v>
@@ -8509,49 +8462,49 @@
         <f>K13-K11</f>
         <v>0.22022022022021426</v>
       </c>
-      <c r="L12" s="99">
+      <c r="L12" s="98">
         <v>450</v>
       </c>
-      <c r="N12" s="139" t="s">
+      <c r="N12" s="170" t="s">
         <v>34</v>
       </c>
       <c r="O12" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="145">
+      <c r="P12" s="179">
         <f>(G13*G15/1000)/0.55</f>
         <v>0.30084630084630076</v>
       </c>
-      <c r="Q12" s="145"/>
-      <c r="R12" s="123">
+      <c r="Q12" s="179"/>
+      <c r="R12" s="121">
         <f>(I13*I15/1000)/0.55</f>
         <v>0.33124033124033125</v>
       </c>
-      <c r="S12" s="123">
+      <c r="S12" s="121">
         <f>(J13*J15/1000)/0.55</f>
         <v>0.21010101010101007</v>
       </c>
-      <c r="T12" s="123">
+      <c r="T12" s="121">
         <f>(K13*K15/1000)/0.55</f>
         <v>1.4196014196013811E-3</v>
       </c>
-      <c r="U12" s="125">
+      <c r="U12" s="123">
         <f>SUM(P12:T12)</f>
         <v>0.8436072436072436</v>
       </c>
       <c r="Y12" s="27"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D13" s="97"/>
-      <c r="E13" s="140"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="171"/>
       <c r="F13" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="148">
+      <c r="G13" s="168">
         <f>((G37+H37)/(1-L37))*$E$2</f>
         <v>570.57057057057045</v>
       </c>
-      <c r="H13" s="148"/>
+      <c r="H13" s="168"/>
       <c r="I13" s="87">
         <f>(I37/(1-L37))*$E$2</f>
         <v>280.28028028028029</v>
@@ -8564,18 +8517,18 @@
         <f>(K37/(1-L37))*$E$2</f>
         <v>1.001001001000974</v>
       </c>
-      <c r="L13" s="100">
+      <c r="L13" s="99">
         <f>SUM(G13:K13)</f>
         <v>999.99999999999989</v>
       </c>
-      <c r="N13" s="140"/>
+      <c r="N13" s="171"/>
       <c r="O13" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="143" t="s">
+      <c r="P13" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="Q13" s="143"/>
+      <c r="Q13" s="167"/>
       <c r="R13" s="84" t="s">
         <v>52</v>
       </c>
@@ -8591,92 +8544,92 @@
       <c r="Y13" s="27"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D14" s="97"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="91"/>
-      <c r="F14" s="113" t="s">
+      <c r="F14" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="149">
+      <c r="G14" s="169">
         <f>G13/$L$7</f>
         <v>0.57057057057057048</v>
       </c>
-      <c r="H14" s="149"/>
-      <c r="I14" s="112">
+      <c r="H14" s="169"/>
+      <c r="I14" s="111">
         <f t="shared" ref="I14" si="6">I13/$L$7</f>
         <v>0.28028028028028029</v>
       </c>
-      <c r="J14" s="112">
+      <c r="J14" s="111">
         <f t="shared" ref="J14" si="7">J13/$L$7</f>
         <v>0.14814814814814814</v>
       </c>
-      <c r="K14" s="112">
+      <c r="K14" s="111">
         <f t="shared" ref="K14" si="8">K13/$L$7</f>
         <v>1.0010010010009741E-3</v>
       </c>
-      <c r="L14" s="101">
+      <c r="L14" s="100">
         <f>SUM(G14:K14)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="N14" s="141"/>
-      <c r="O14" s="119" t="s">
+      <c r="N14" s="178"/>
+      <c r="O14" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="P14" s="144"/>
-      <c r="Q14" s="144"/>
-      <c r="R14" s="120"/>
-      <c r="S14" s="120"/>
-      <c r="T14" s="120"/>
-      <c r="U14" s="121"/>
+      <c r="P14" s="174"/>
+      <c r="Q14" s="174"/>
+      <c r="R14" s="118"/>
+      <c r="S14" s="118"/>
+      <c r="T14" s="118"/>
+      <c r="U14" s="119"/>
       <c r="Y14" s="27"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D15" s="97"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="92"/>
       <c r="F15" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="153">
+      <c r="G15" s="164">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H15" s="153"/>
-      <c r="I15" s="124">
+      <c r="H15" s="164"/>
+      <c r="I15" s="122">
         <v>0.65</v>
       </c>
-      <c r="J15" s="124">
+      <c r="J15" s="122">
         <v>0.78</v>
       </c>
-      <c r="K15" s="124">
+      <c r="K15" s="122">
         <v>0.78</v>
       </c>
-      <c r="L15" s="102"/>
+      <c r="L15" s="101"/>
       <c r="Y15" s="27"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D16" s="97"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="83"/>
       <c r="F16" s="83"/>
       <c r="G16" s="84"/>
       <c r="H16" s="84"/>
       <c r="I16" s="84"/>
       <c r="J16" s="84"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="104"/>
       <c r="P16" s="27"/>
       <c r="Y16" s="27"/>
     </row>
     <row r="17" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D17" s="97"/>
-      <c r="E17" s="139" t="s">
+      <c r="D17" s="96"/>
+      <c r="E17" s="170" t="s">
         <v>35</v>
       </c>
       <c r="F17" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="154">
+      <c r="G17" s="166">
         <f>L17-K17-J17-I17</f>
         <v>179.42828485456371</v>
       </c>
-      <c r="H17" s="154"/>
+      <c r="H17" s="166"/>
       <c r="I17" s="82">
         <f>I21*I19</f>
         <v>208.62587763289869</v>
@@ -8689,42 +8642,42 @@
         <f t="shared" si="9"/>
         <v>5.4764292878635423</v>
       </c>
-      <c r="L17" s="98">
+      <c r="L17" s="97">
         <v>550</v>
       </c>
-      <c r="N17" s="114" t="s">
+      <c r="N17" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="115"/>
-      <c r="P17" s="138" t="s">
+      <c r="O17" s="114"/>
+      <c r="P17" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="138"/>
-      <c r="R17" s="116" t="s">
+      <c r="Q17" s="177"/>
+      <c r="R17" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="S17" s="116" t="s">
+      <c r="S17" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="T17" s="116" t="s">
+      <c r="T17" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="U17" s="117"/>
+      <c r="U17" s="116"/>
       <c r="Y17" s="27"/>
       <c r="Z17" s="27"/>
       <c r="AA17" s="27"/>
     </row>
     <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="48"/>
-      <c r="E18" s="140"/>
+      <c r="E18" s="171"/>
       <c r="F18" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="143">
+      <c r="G18" s="167">
         <f>G19-G17</f>
         <v>291.98595787362081</v>
       </c>
-      <c r="H18" s="143"/>
+      <c r="H18" s="167"/>
       <c r="I18" s="84">
         <f t="shared" ref="I18" si="10">I19-I17</f>
         <v>112.33701103309929</v>
@@ -8737,48 +8690,48 @@
         <f>K19-K17</f>
         <v>1.544633901705101</v>
       </c>
-      <c r="L18" s="99">
+      <c r="L18" s="98">
         <v>450</v>
       </c>
-      <c r="N18" s="139" t="s">
+      <c r="N18" s="170" t="s">
         <v>35</v>
       </c>
       <c r="O18" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P18" s="142">
+      <c r="P18" s="180">
         <f>(G19*G21/1000)/0.55</f>
         <v>0.32623324519011582</v>
       </c>
-      <c r="Q18" s="142"/>
-      <c r="R18" s="122">
+      <c r="Q18" s="180"/>
+      <c r="R18" s="120">
         <f>(I19*I21/1000)/0.55</f>
         <v>0.37931977751436124</v>
       </c>
-      <c r="S18" s="122">
+      <c r="S18" s="120">
         <f>(J19*J21/1000)/0.55</f>
         <v>0.28448983313577098</v>
       </c>
-      <c r="T18" s="122">
+      <c r="T18" s="120">
         <f>(K19*K21/1000)/0.55</f>
         <v>9.9571441597518951E-3</v>
       </c>
-      <c r="U18" s="125">
+      <c r="U18" s="123">
         <f>SUM(P18:T18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="48"/>
-      <c r="E19" s="140"/>
+      <c r="E19" s="171"/>
       <c r="F19" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="148">
+      <c r="G19" s="168">
         <f>((G38+H38)/(1-L38))*$E$2</f>
         <v>471.41424272818455</v>
       </c>
-      <c r="H19" s="148"/>
+      <c r="H19" s="168"/>
       <c r="I19" s="87">
         <f>(I38/(1-L38))*$E$2</f>
         <v>320.96288866599798</v>
@@ -8791,18 +8744,18 @@
         <f>(K38/(1-L38))*$E$2</f>
         <v>7.0210631895686433</v>
       </c>
-      <c r="L19" s="100">
+      <c r="L19" s="99">
         <f>SUM(G19:K19)</f>
         <v>999.99999999999989</v>
       </c>
-      <c r="N19" s="140"/>
+      <c r="N19" s="171"/>
       <c r="O19" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="143" t="s">
+      <c r="P19" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" s="143"/>
+      <c r="Q19" s="167"/>
       <c r="R19" s="84" t="s">
         <v>52</v>
       </c>
@@ -8819,40 +8772,40 @@
     <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="48"/>
       <c r="E20" s="88"/>
-      <c r="F20" s="113" t="s">
+      <c r="F20" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="149">
+      <c r="G20" s="169">
         <f>G19/$L$7</f>
         <v>0.47141424272818455</v>
       </c>
-      <c r="H20" s="149"/>
-      <c r="I20" s="112">
+      <c r="H20" s="169"/>
+      <c r="I20" s="111">
         <f t="shared" ref="I20" si="12">I19/$L$7</f>
         <v>0.32096288866599798</v>
       </c>
-      <c r="J20" s="112">
+      <c r="J20" s="111">
         <f t="shared" ref="J20" si="13">J19/$L$7</f>
         <v>0.20060180541624878</v>
       </c>
-      <c r="K20" s="112">
+      <c r="K20" s="111">
         <f t="shared" ref="K20" si="14">K19/$L$7</f>
         <v>7.021063189568643E-3</v>
       </c>
-      <c r="L20" s="101">
+      <c r="L20" s="100">
         <f>SUM(G20:K20)</f>
         <v>1</v>
       </c>
-      <c r="N20" s="141"/>
-      <c r="O20" s="119" t="s">
+      <c r="N20" s="178"/>
+      <c r="O20" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="P20" s="144"/>
-      <c r="Q20" s="144"/>
-      <c r="R20" s="120"/>
-      <c r="S20" s="120"/>
-      <c r="T20" s="120"/>
-      <c r="U20" s="121"/>
+      <c r="P20" s="174"/>
+      <c r="Q20" s="174"/>
+      <c r="R20" s="118"/>
+      <c r="S20" s="118"/>
+      <c r="T20" s="118"/>
+      <c r="U20" s="119"/>
     </row>
     <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="48"/>
@@ -8860,21 +8813,21 @@
       <c r="F21" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="153">
+      <c r="G21" s="164">
         <f>G17/G19</f>
         <v>0.3806170212765958</v>
       </c>
-      <c r="H21" s="153"/>
-      <c r="I21" s="124">
+      <c r="H21" s="164"/>
+      <c r="I21" s="122">
         <v>0.65</v>
       </c>
-      <c r="J21" s="124">
+      <c r="J21" s="122">
         <v>0.78</v>
       </c>
-      <c r="K21" s="124">
+      <c r="K21" s="122">
         <v>0.78</v>
       </c>
-      <c r="L21" s="102"/>
+      <c r="L21" s="101"/>
     </row>
     <row r="22" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D22" s="48"/>
@@ -8885,21 +8838,21 @@
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
-      <c r="L22" s="105"/>
+      <c r="L22" s="104"/>
     </row>
     <row r="23" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D23" s="48"/>
-      <c r="E23" s="151" t="s">
+      <c r="E23" s="172" t="s">
         <v>36</v>
       </c>
       <c r="F23" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="154">
+      <c r="G23" s="166">
         <f>L23-K23-J23-I23</f>
         <v>150.20100502512565</v>
       </c>
-      <c r="H23" s="154"/>
+      <c r="H23" s="166"/>
       <c r="I23" s="82">
         <f>I27*I25</f>
         <v>215.5778894472362</v>
@@ -8912,39 +8865,39 @@
         <f t="shared" si="15"/>
         <v>3.919597989949736</v>
       </c>
-      <c r="L23" s="98">
+      <c r="L23" s="97">
         <v>550</v>
       </c>
-      <c r="N23" s="114" t="s">
+      <c r="N23" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="O23" s="115"/>
-      <c r="P23" s="138" t="s">
+      <c r="O23" s="114"/>
+      <c r="P23" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="Q23" s="138"/>
-      <c r="R23" s="116" t="s">
+      <c r="Q23" s="177"/>
+      <c r="R23" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="S23" s="116" t="s">
+      <c r="S23" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="T23" s="116" t="s">
+      <c r="T23" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="U23" s="117"/>
+      <c r="U23" s="116"/>
     </row>
     <row r="24" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D24" s="48"/>
-      <c r="E24" s="152"/>
+      <c r="E24" s="173"/>
       <c r="F24" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="143">
+      <c r="G24" s="167">
         <f>G25-G23</f>
         <v>281.95979899497485</v>
       </c>
-      <c r="H24" s="143"/>
+      <c r="H24" s="167"/>
       <c r="I24" s="84">
         <f t="shared" ref="I24" si="16">I25-I23</f>
         <v>116.08040201005025</v>
@@ -8957,48 +8910,48 @@
         <f>K25-K23</f>
         <v>1.1055276381909511</v>
       </c>
-      <c r="L24" s="99">
+      <c r="L24" s="98">
         <v>450</v>
       </c>
-      <c r="N24" s="139" t="s">
+      <c r="N24" s="170" t="s">
         <v>36</v>
       </c>
       <c r="O24" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P24" s="142">
+      <c r="P24" s="180">
         <f>(G25*G27/1000)/0.55</f>
         <v>0.27309273640931936</v>
       </c>
-      <c r="Q24" s="142"/>
-      <c r="R24" s="122">
+      <c r="Q24" s="180"/>
+      <c r="R24" s="120">
         <f>(I25*I27/1000)/0.55</f>
         <v>0.39195979899497491</v>
       </c>
-      <c r="S24" s="122">
+      <c r="S24" s="120">
         <f>(J25*J27/1000)/0.55</f>
         <v>0.32782092279579716</v>
       </c>
-      <c r="T24" s="122">
+      <c r="T24" s="120">
         <f>(K25*K27/1000)/0.55</f>
         <v>7.1265417999086108E-3</v>
       </c>
-      <c r="U24" s="125">
+      <c r="U24" s="123">
         <f>SUM(P24:T24)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="25" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D25" s="48"/>
-      <c r="E25" s="152"/>
+      <c r="E25" s="173"/>
       <c r="F25" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="148">
+      <c r="G25" s="168">
         <f>((G39+H39)/(1-L39))*$E$2</f>
         <v>432.1608040201005</v>
       </c>
-      <c r="H25" s="148"/>
+      <c r="H25" s="168"/>
       <c r="I25" s="87">
         <f>(I39/(1-L39))*$E$2</f>
         <v>331.65829145728645</v>
@@ -9011,18 +8964,18 @@
         <f>(K39/(1-L39))*$E$2</f>
         <v>5.0251256281406871</v>
       </c>
-      <c r="L25" s="100">
+      <c r="L25" s="99">
         <f>SUM(G25:K25)</f>
         <v>1000.0000000000001</v>
       </c>
-      <c r="N25" s="140"/>
+      <c r="N25" s="171"/>
       <c r="O25" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="143" t="s">
+      <c r="P25" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="Q25" s="143"/>
+      <c r="Q25" s="167"/>
       <c r="R25" s="84" t="s">
         <v>52</v>
       </c>
@@ -9039,40 +8992,40 @@
     <row r="26" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D26" s="48"/>
       <c r="E26" s="88"/>
-      <c r="F26" s="113" t="s">
+      <c r="F26" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="149">
+      <c r="G26" s="169">
         <f>G25/$L$7</f>
         <v>0.43216080402010049</v>
       </c>
-      <c r="H26" s="149"/>
-      <c r="I26" s="112">
+      <c r="H26" s="169"/>
+      <c r="I26" s="111">
         <f t="shared" ref="I26" si="18">I25/$L$7</f>
         <v>0.33165829145728642</v>
       </c>
-      <c r="J26" s="112">
+      <c r="J26" s="111">
         <f t="shared" ref="J26" si="19">J25/$L$7</f>
         <v>0.23115577889447236</v>
       </c>
-      <c r="K26" s="112">
+      <c r="K26" s="111">
         <f t="shared" ref="K26" si="20">K25/$L$7</f>
         <v>5.0251256281406871E-3</v>
       </c>
-      <c r="L26" s="101">
+      <c r="L26" s="100">
         <f>SUM(G26:K26)</f>
         <v>1</v>
       </c>
-      <c r="N26" s="141"/>
-      <c r="O26" s="119" t="s">
+      <c r="N26" s="178"/>
+      <c r="O26" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="P26" s="144"/>
-      <c r="Q26" s="144"/>
-      <c r="R26" s="120"/>
-      <c r="S26" s="120"/>
-      <c r="T26" s="120"/>
-      <c r="U26" s="121"/>
+      <c r="P26" s="174"/>
+      <c r="Q26" s="174"/>
+      <c r="R26" s="118"/>
+      <c r="S26" s="118"/>
+      <c r="T26" s="118"/>
+      <c r="U26" s="119"/>
     </row>
     <row r="27" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D27" s="48"/>
@@ -9080,24 +9033,24 @@
       <c r="F27" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="153">
+      <c r="G27" s="164">
         <f>G23/G25</f>
         <v>0.34755813953488379</v>
       </c>
-      <c r="H27" s="153"/>
-      <c r="I27" s="124">
+      <c r="H27" s="164"/>
+      <c r="I27" s="122">
         <v>0.65</v>
       </c>
-      <c r="J27" s="124">
+      <c r="J27" s="122">
         <v>0.78</v>
       </c>
-      <c r="K27" s="124">
+      <c r="K27" s="122">
         <v>0.78</v>
       </c>
-      <c r="L27" s="102"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D28" s="97"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="83"/>
       <c r="F28" s="35"/>
       <c r="G28" s="83"/>
@@ -9105,21 +9058,21 @@
       <c r="I28" s="83"/>
       <c r="J28" s="83"/>
       <c r="K28" s="83"/>
-      <c r="L28" s="107"/>
+      <c r="L28" s="106"/>
     </row>
     <row r="29" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D29" s="97"/>
-      <c r="E29" s="151" t="s">
+      <c r="D29" s="96"/>
+      <c r="E29" s="172" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="154">
+      <c r="G29" s="166">
         <f>L29-K29-J29-I29</f>
         <v>180.18145161290317</v>
       </c>
-      <c r="H29" s="154"/>
+      <c r="H29" s="166"/>
       <c r="I29" s="82">
         <f>I33*I31</f>
         <v>203.125</v>
@@ -9132,39 +9085,39 @@
         <f t="shared" si="21"/>
         <v>17.298387096774238</v>
       </c>
-      <c r="L29" s="98">
+      <c r="L29" s="97">
         <v>550</v>
       </c>
-      <c r="N29" s="114" t="s">
+      <c r="N29" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="O29" s="115"/>
-      <c r="P29" s="138" t="s">
+      <c r="O29" s="114"/>
+      <c r="P29" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="Q29" s="138"/>
-      <c r="R29" s="116" t="s">
+      <c r="Q29" s="177"/>
+      <c r="R29" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="S29" s="116" t="s">
+      <c r="S29" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="T29" s="116" t="s">
+      <c r="T29" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="U29" s="117"/>
+      <c r="U29" s="116"/>
     </row>
     <row r="30" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D30" s="97"/>
-      <c r="E30" s="152"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="173"/>
       <c r="F30" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="143">
+      <c r="G30" s="167">
         <f>G31-G29</f>
         <v>293.60887096774195</v>
       </c>
-      <c r="H30" s="143"/>
+      <c r="H30" s="167"/>
       <c r="I30" s="84">
         <f t="shared" ref="I30" si="22">I31-I29</f>
         <v>109.375</v>
@@ -9177,48 +9130,48 @@
         <f>K31-K29</f>
         <v>4.8790322580645302</v>
       </c>
-      <c r="L30" s="99">
+      <c r="L30" s="98">
         <v>450</v>
       </c>
-      <c r="N30" s="139" t="s">
+      <c r="N30" s="170" t="s">
         <v>37</v>
       </c>
       <c r="O30" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="P30" s="142">
+      <c r="P30" s="180">
         <f>(G31*G33/1000)/0.55</f>
         <v>0.32760263929618755</v>
       </c>
-      <c r="Q30" s="142"/>
-      <c r="R30" s="122">
+      <c r="Q30" s="180"/>
+      <c r="R30" s="120">
         <f>(I31*I33/1000)/0.55</f>
         <v>0.36931818181818177</v>
       </c>
-      <c r="S30" s="122">
+      <c r="S30" s="120">
         <f>(J31*J33/1000)/0.55</f>
         <v>0.27162756598240473</v>
       </c>
-      <c r="T30" s="122">
+      <c r="T30" s="120">
         <f>(K31*K33/1000)/0.55</f>
         <v>3.1451612903225887E-2</v>
       </c>
-      <c r="U30" s="125">
+      <c r="U30" s="123">
         <f>SUM(P30:T30)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D31" s="97"/>
-      <c r="E31" s="152"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="173"/>
       <c r="F31" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="148">
+      <c r="G31" s="168">
         <f>((G40+H40)/(1-L40))*$E$2</f>
         <v>473.79032258064512</v>
       </c>
-      <c r="H31" s="148"/>
+      <c r="H31" s="168"/>
       <c r="I31" s="87">
         <f>(I40/(1-L40))*$E$2</f>
         <v>312.5</v>
@@ -9231,18 +9184,18 @@
         <f>(K40/(1-L40))*$E$2</f>
         <v>22.177419354838769</v>
       </c>
-      <c r="L31" s="100">
+      <c r="L31" s="99">
         <f>SUM(G31:K31)</f>
         <v>1000</v>
       </c>
-      <c r="N31" s="140"/>
+      <c r="N31" s="171"/>
       <c r="O31" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="P31" s="143" t="s">
+      <c r="P31" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="Q31" s="143"/>
+      <c r="Q31" s="167"/>
       <c r="R31" s="84" t="s">
         <v>52</v>
       </c>
@@ -9257,64 +9210,64 @@
       </c>
     </row>
     <row r="32" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D32" s="97"/>
+      <c r="D32" s="96"/>
       <c r="E32" s="88"/>
-      <c r="F32" s="113" t="s">
+      <c r="F32" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="149">
+      <c r="G32" s="169">
         <f>G31/$L$7</f>
         <v>0.47379032258064513</v>
       </c>
-      <c r="H32" s="149"/>
-      <c r="I32" s="112">
+      <c r="H32" s="169"/>
+      <c r="I32" s="111">
         <f t="shared" ref="I32" si="24">I31/$L$7</f>
         <v>0.3125</v>
       </c>
-      <c r="J32" s="112">
+      <c r="J32" s="111">
         <f t="shared" ref="J32" si="25">J31/$L$7</f>
         <v>0.19153225806451613</v>
       </c>
-      <c r="K32" s="112">
+      <c r="K32" s="111">
         <f t="shared" ref="K32" si="26">K31/$L$7</f>
         <v>2.217741935483877E-2</v>
       </c>
-      <c r="L32" s="101">
+      <c r="L32" s="100">
         <f>SUM(G32:K32)</f>
         <v>1</v>
       </c>
-      <c r="N32" s="141"/>
-      <c r="O32" s="119" t="s">
+      <c r="N32" s="178"/>
+      <c r="O32" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="P32" s="144"/>
-      <c r="Q32" s="144"/>
-      <c r="R32" s="120"/>
-      <c r="S32" s="120"/>
-      <c r="T32" s="120"/>
-      <c r="U32" s="121"/>
+      <c r="P32" s="174"/>
+      <c r="Q32" s="174"/>
+      <c r="R32" s="118"/>
+      <c r="S32" s="118"/>
+      <c r="T32" s="118"/>
+      <c r="U32" s="119"/>
     </row>
     <row r="33" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="49"/>
-      <c r="E33" s="108"/>
-      <c r="F33" s="109" t="s">
+      <c r="E33" s="107"/>
+      <c r="F33" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="150">
+      <c r="G33" s="181">
         <f>G29/G31</f>
         <v>0.38029787234042545</v>
       </c>
-      <c r="H33" s="150"/>
-      <c r="I33" s="124">
+      <c r="H33" s="181"/>
+      <c r="I33" s="122">
         <v>0.65</v>
       </c>
-      <c r="J33" s="124">
+      <c r="J33" s="122">
         <v>0.78</v>
       </c>
-      <c r="K33" s="124">
+      <c r="K33" s="122">
         <v>0.78</v>
       </c>
-      <c r="L33" s="110"/>
+      <c r="L33" s="109"/>
     </row>
     <row r="34" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="63"/>
@@ -9326,7 +9279,7 @@
       <c r="L34" s="64"/>
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D35" s="111" t="s">
+      <c r="D35" s="110" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="45" t="s">
@@ -9354,7 +9307,7 @@
       <c r="M35" s="27"/>
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D36" s="146" t="s">
+      <c r="D36" s="175" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="28" t="s">
@@ -9381,7 +9334,7 @@
       </c>
     </row>
     <row r="37" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D37" s="146"/>
+      <c r="D37" s="175"/>
       <c r="E37" s="28" t="s">
         <v>34</v>
       </c>
@@ -9406,7 +9359,7 @@
       </c>
     </row>
     <row r="38" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D38" s="146"/>
+      <c r="D38" s="175"/>
       <c r="E38" s="28" t="s">
         <v>35</v>
       </c>
@@ -9431,7 +9384,7 @@
       </c>
     </row>
     <row r="39" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D39" s="146"/>
+      <c r="D39" s="175"/>
       <c r="E39" s="28" t="s">
         <v>36</v>
       </c>
@@ -9456,7 +9409,7 @@
       </c>
     </row>
     <row r="40" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="147"/>
+      <c r="D40" s="176"/>
       <c r="E40" s="77" t="s">
         <v>37</v>
       </c>
@@ -9504,32 +9457,22 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N24:N26"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="D36:D40"/>
     <mergeCell ref="P4:Q4"/>
@@ -9546,22 +9489,32 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="N2:U2"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="N24:N26"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9569,12 +9522,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U55"/>
+  <dimension ref="B1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9599,21 +9552,21 @@
         <v>2</v>
       </c>
       <c r="D2" s="72"/>
-      <c r="E2" s="95" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="157" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="132" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132" t="s">
-        <v>119</v>
+      <c r="E2" s="139" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="139" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="141" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130" t="s">
+        <v>101</v>
       </c>
       <c r="R2" s="61" t="s">
         <v>31</v>
@@ -9623,34 +9576,32 @@
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="139" t="s">
-        <v>97</v>
+      <c r="C3" s="170" t="s">
+        <v>107</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="166">
+      <c r="E3" s="149">
         <f>E7*E5</f>
-        <v>73.8</v>
-      </c>
-      <c r="F3" s="167">
+        <v>0</v>
+      </c>
+      <c r="F3" s="150">
         <f>G3-E3</f>
-        <v>490.2</v>
-      </c>
-      <c r="G3" s="170">
-        <v>564</v>
-      </c>
-      <c r="H3" s="182">
-        <f>(E3/F3)/(E4/F4)</f>
-        <v>3.9013101228523492</v>
-      </c>
-      <c r="I3" s="182"/>
-      <c r="J3" s="1">
-        <f>(E3/(E3+F3))/(E4/(E4+F4))</f>
-        <v>3.521670606776989</v>
+        <v>4397</v>
+      </c>
+      <c r="G3" s="152">
+        <v>4397</v>
+      </c>
+      <c r="H3" s="161" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="161"/>
+      <c r="J3" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="R3" s="61" t="s">
         <v>32</v>
@@ -9660,47 +9611,47 @@
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="140"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="171"/>
       <c r="D4" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="136">
         <f>E5-E3</f>
-        <v>16.200000000000003</v>
-      </c>
-      <c r="F4" s="168">
+        <v>0</v>
+      </c>
+      <c r="F4" s="151">
         <f>G4-E4</f>
-        <v>419.8</v>
-      </c>
-      <c r="G4" s="170">
+        <v>5603</v>
+      </c>
+      <c r="G4" s="152">
         <f>G5-G3</f>
-        <v>436</v>
-      </c>
-      <c r="H4" s="182"/>
-      <c r="I4" s="182"/>
+        <v>5603</v>
+      </c>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
       <c r="R4" s="61"/>
       <c r="S4" s="60"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="48"/>
-      <c r="C5" s="140"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="180">
+      <c r="E5" s="160">
         <f>E6*G5</f>
-        <v>90</v>
-      </c>
-      <c r="F5" s="178">
+        <v>0</v>
+      </c>
+      <c r="F5" s="158">
         <f>F6*G5</f>
-        <v>910</v>
-      </c>
-      <c r="G5" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
+        <v>10000</v>
+      </c>
+      <c r="G5" s="152">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
       <c r="R5" s="61" t="s">
         <v>46</v>
       </c>
@@ -9708,21 +9659,21 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="48"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="181">
-        <f>(0.5*E42)+(0.5*E50)</f>
-        <v>0.09</v>
-      </c>
-      <c r="F6" s="179">
+      <c r="C6" s="134"/>
+      <c r="D6" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="188">
+        <f>E35/100</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="159">
         <f>1-E6</f>
-        <v>0.91</v>
-      </c>
-      <c r="G6" s="105"/>
-      <c r="H6" s="182"/>
-      <c r="I6" s="182"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="104"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
       <c r="R6" s="27"/>
       <c r="S6" s="60" t="s">
         <v>26</v>
@@ -9730,70 +9681,65 @@
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="48"/>
-      <c r="C7" s="118"/>
+      <c r="C7" s="135"/>
       <c r="D7" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="183">
-        <v>0.82</v>
-      </c>
-      <c r="F7" s="164">
-        <f>F3/F5</f>
-        <v>0.53868131868131863</v>
-      </c>
-      <c r="G7" s="105"/>
-      <c r="H7" s="182"/>
-      <c r="I7" s="182"/>
+        <v>102</v>
+      </c>
+      <c r="E7" s="162"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
       <c r="R7" s="27"/>
       <c r="S7" s="60"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="48"/>
-      <c r="C8" s="97"/>
+      <c r="C8" s="137"/>
       <c r="D8" s="83"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="182"/>
-      <c r="I8" s="182"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="161"/>
+      <c r="I8" s="161"/>
       <c r="R8" s="27" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="S8" s="1">
         <v>3.8</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="97"/>
-      <c r="C9" s="169" t="s">
-        <v>98</v>
+      <c r="B9" s="137"/>
+      <c r="C9" s="185" t="s">
+        <v>108</v>
       </c>
       <c r="D9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="166">
+      <c r="E9" s="149">
         <f>E13*E11</f>
-        <v>93.149999999999991</v>
-      </c>
-      <c r="F9" s="167">
+        <v>38.249999999999986</v>
+      </c>
+      <c r="F9" s="150">
         <f>G9-E9</f>
-        <v>470.85</v>
-      </c>
-      <c r="G9" s="170">
-        <v>564</v>
-      </c>
-      <c r="H9" s="182">
+        <v>4358.75</v>
+      </c>
+      <c r="G9" s="152">
+        <v>4397</v>
+      </c>
+      <c r="H9" s="161">
         <f>(E9/F9)/(E10/F10)</f>
-        <v>3.7497862208883155</v>
-      </c>
-      <c r="I9" s="182"/>
+        <v>3.8476053914539703</v>
+      </c>
+      <c r="I9" s="161"/>
       <c r="J9" s="1">
         <f>(E9/(E9+F9))/(E10/(E10+F10))</f>
-        <v>3.2956326987681979</v>
+        <v>3.8228337502842837</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
@@ -9801,199 +9747,205 @@
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="97"/>
-      <c r="C10" s="146"/>
+      <c r="B10" s="137"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="84">
+      <c r="E10" s="136">
         <f>E11-E9</f>
-        <v>21.849999999999994</v>
-      </c>
-      <c r="F10" s="168">
+        <v>12.75</v>
+      </c>
+      <c r="F10" s="151">
         <f>G10-E10</f>
-        <v>414.15</v>
-      </c>
-      <c r="G10" s="170">
+        <v>5590.25</v>
+      </c>
+      <c r="G10" s="152">
         <f>G11-G9</f>
-        <v>436</v>
-      </c>
-      <c r="H10" s="182"/>
-      <c r="I10" s="182"/>
+        <v>5603</v>
+      </c>
+      <c r="H10" s="161">
+        <f>(E9/E10)/(F9/F10)</f>
+        <v>3.8476053914539703</v>
+      </c>
+      <c r="I10" s="161"/>
       <c r="R10" s="27"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="97"/>
-      <c r="C11" s="146"/>
+      <c r="B11" s="137"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="162">
+      <c r="E11" s="145">
         <f>E12*G11</f>
-        <v>114.99999999999999</v>
-      </c>
-      <c r="F11" s="165">
+        <v>50.999999999999986</v>
+      </c>
+      <c r="F11" s="148">
         <f>F12*G11</f>
-        <v>885</v>
-      </c>
-      <c r="G11" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="182"/>
-      <c r="I11" s="182"/>
+        <v>9949</v>
+      </c>
+      <c r="G11" s="152">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="161">
-        <f>(0.5*E43)+(0.5*E51)</f>
-        <v>0.11499999999999999</v>
-      </c>
-      <c r="F12" s="163">
+      <c r="B12" s="137"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="189">
+        <f>E36/100</f>
+        <v>5.0999999999999986E-3</v>
+      </c>
+      <c r="F12" s="146">
         <f>1-E12</f>
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="G12" s="105"/>
-      <c r="H12" s="182"/>
-      <c r="I12" s="182"/>
+        <v>0.99490000000000001</v>
+      </c>
+      <c r="G12" s="104"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="161"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="97"/>
-      <c r="C13" s="171"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="153"/>
       <c r="D13" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" s="183">
-        <v>0.81</v>
-      </c>
-      <c r="F13" s="164">
+        <v>102</v>
+      </c>
+      <c r="E13" s="191">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="147">
         <f>F9/F11</f>
-        <v>0.53203389830508474</v>
-      </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="182"/>
+        <v>0.43810935772439441</v>
+      </c>
+      <c r="G13" s="104"/>
+      <c r="H13" s="161"/>
+      <c r="I13" s="161"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
       <c r="D14" s="83"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="182"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="136"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="161"/>
+      <c r="I14" s="161"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="97"/>
-      <c r="C15" s="169" t="s">
-        <v>33</v>
+      <c r="B15" s="137"/>
+      <c r="C15" s="185" t="s">
+        <v>111</v>
       </c>
       <c r="D15" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="166">
+      <c r="E15" s="149">
         <f>E19*E17</f>
-        <v>73.8</v>
-      </c>
-      <c r="F15" s="167">
+        <v>108.75</v>
+      </c>
+      <c r="F15" s="150">
         <f>G15-E15</f>
-        <v>490.2</v>
-      </c>
-      <c r="G15" s="170">
-        <v>564</v>
-      </c>
-      <c r="H15" s="182">
+        <v>4288.25</v>
+      </c>
+      <c r="G15" s="152">
+        <v>4397</v>
+      </c>
+      <c r="H15" s="161">
         <f>(E15/F15)/(E16/F16)</f>
-        <v>3.9013101228523492</v>
-      </c>
-      <c r="I15" s="182"/>
+        <v>3.8944208010260599</v>
+      </c>
+      <c r="I15" s="161"/>
       <c r="J15" s="1">
         <f>(E15/(E15+F15))/(E16/(E16+F16))</f>
-        <v>3.521670606776989</v>
+        <v>3.8228337502842846</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="48"/>
-      <c r="C16" s="146"/>
+      <c r="C16" s="175"/>
       <c r="D16" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="84">
+      <c r="E16" s="136">
         <f>E17-E15</f>
-        <v>16.200000000000003</v>
-      </c>
-      <c r="F16" s="168">
+        <v>36.25</v>
+      </c>
+      <c r="F16" s="151">
         <f>G16-E16</f>
-        <v>419.8</v>
-      </c>
-      <c r="G16" s="170">
+        <v>5566.75</v>
+      </c>
+      <c r="G16" s="152">
         <f>G17-G15</f>
-        <v>436</v>
-      </c>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
+        <v>5603</v>
+      </c>
+      <c r="H16" s="161">
+        <f>(E15/E16)/(F15/F16)</f>
+        <v>3.8944208010260595</v>
+      </c>
+      <c r="I16" s="161"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="48"/>
-      <c r="C17" s="146"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="162">
+      <c r="E17" s="145">
         <f>E18*G17</f>
-        <v>90</v>
-      </c>
-      <c r="F17" s="165">
+        <v>145</v>
+      </c>
+      <c r="F17" s="148">
         <f>F18*G17</f>
-        <v>910</v>
-      </c>
-      <c r="G17" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
+        <v>9855</v>
+      </c>
+      <c r="G17" s="152">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="48"/>
       <c r="C18" s="46"/>
-      <c r="D18" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="161">
-        <f>(0.5*E44)+(0.5*E52)</f>
-        <v>0.09</v>
-      </c>
-      <c r="F18" s="163">
+      <c r="D18" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="189">
+        <f>E37/100</f>
+        <v>1.4499999999999999E-2</v>
+      </c>
+      <c r="F18" s="146">
         <f>1-E18</f>
-        <v>0.91</v>
-      </c>
-      <c r="G18" s="105"/>
-      <c r="H18" s="182"/>
-      <c r="I18" s="182"/>
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="G18" s="104"/>
+      <c r="H18" s="161"/>
+      <c r="I18" s="161"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="48"/>
-      <c r="C19" s="172"/>
+      <c r="C19" s="154"/>
       <c r="D19" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="E19" s="183">
-        <v>0.82</v>
-      </c>
-      <c r="F19" s="164">
+        <v>102</v>
+      </c>
+      <c r="E19" s="191">
+        <v>0.75</v>
+      </c>
+      <c r="F19" s="147">
         <f>F15/F17</f>
-        <v>0.53868131868131863</v>
-      </c>
-      <c r="G19" s="105"/>
-      <c r="H19" s="182"/>
-      <c r="I19" s="182"/>
+        <v>0.43513444951801117</v>
+      </c>
+      <c r="G19" s="104"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="48"/>
@@ -10001,572 +9953,352 @@
       <c r="D20" s="35"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="48"/>
-      <c r="C21" s="173" t="s">
-        <v>34</v>
+      <c r="C21" s="183" t="s">
+        <v>113</v>
       </c>
       <c r="D21" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="166">
+      <c r="E21" s="149">
         <f>E25*E23</f>
-        <v>113.4</v>
-      </c>
-      <c r="F21" s="167">
+        <v>305.61999999999995</v>
+      </c>
+      <c r="F21" s="150">
         <f>G21-E21</f>
-        <v>450.6</v>
-      </c>
-      <c r="G21" s="170">
-        <v>564</v>
-      </c>
-      <c r="H21" s="182">
+        <v>4091.38</v>
+      </c>
+      <c r="G21" s="152">
+        <v>4397</v>
+      </c>
+      <c r="H21" s="161">
         <f>(E21/F21)/(E22/F22)</f>
-        <v>3.8733618333450148</v>
-      </c>
-      <c r="I21" s="182"/>
+        <v>3.82300837370276</v>
+      </c>
+      <c r="I21" s="161"/>
       <c r="J21" s="1">
         <f>(E21/(E21+F21))/(E22/(E22+F22))</f>
-        <v>3.2956326987681979</v>
+        <v>3.6267909938594491</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="48"/>
-      <c r="C22" s="174"/>
+      <c r="C22" s="184"/>
       <c r="D22" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="84">
+      <c r="E22" s="136">
         <f>E23-E21</f>
-        <v>26.599999999999994</v>
-      </c>
-      <c r="F22" s="168">
+        <v>107.38</v>
+      </c>
+      <c r="F22" s="151">
         <f>G22-E22</f>
-        <v>409.4</v>
-      </c>
-      <c r="G22" s="170">
+        <v>5495.62</v>
+      </c>
+      <c r="G22" s="152">
         <f>G23-G21</f>
-        <v>436</v>
-      </c>
-      <c r="H22" s="182"/>
-      <c r="I22" s="182"/>
+        <v>5603</v>
+      </c>
+      <c r="H22" s="161">
+        <f>(E21/E22)/(F21/F22)</f>
+        <v>3.82300837370276</v>
+      </c>
+      <c r="I22" s="161"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="48"/>
-      <c r="C23" s="174"/>
+      <c r="C23" s="184"/>
       <c r="D23" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="162">
+      <c r="E23" s="145">
         <f>E24*G23</f>
-        <v>140</v>
-      </c>
-      <c r="F23" s="165">
+        <v>412.99999999999994</v>
+      </c>
+      <c r="F23" s="148">
         <f>F24*G23</f>
-        <v>860</v>
-      </c>
-      <c r="G23" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H23" s="182"/>
-      <c r="I23" s="182"/>
+        <v>9587</v>
+      </c>
+      <c r="G23" s="152">
+        <v>10000</v>
+      </c>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="48"/>
       <c r="C24" s="46"/>
-      <c r="D24" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="161">
-        <f>(0.5*E45)+(0.5*E53)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F24" s="163">
+      <c r="D24" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="189">
+        <f>E38/100</f>
+        <v>4.1299999999999996E-2</v>
+      </c>
+      <c r="F24" s="146">
         <f>1-E24</f>
-        <v>0.86</v>
-      </c>
-      <c r="G24" s="105"/>
-      <c r="H24" s="182"/>
-      <c r="I24" s="182"/>
+        <v>0.9587</v>
+      </c>
+      <c r="G24" s="104"/>
+      <c r="H24" s="161"/>
+      <c r="I24" s="161"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="48"/>
-      <c r="C25" s="172"/>
+      <c r="C25" s="154"/>
       <c r="D25" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="E25" s="183">
-        <v>0.81</v>
-      </c>
-      <c r="F25" s="164">
+        <v>102</v>
+      </c>
+      <c r="E25" s="191">
+        <v>0.74</v>
+      </c>
+      <c r="F25" s="147">
         <f>F21/F23</f>
-        <v>0.5239534883720931</v>
-      </c>
-      <c r="G25" s="105"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
+        <v>0.42676332533639305</v>
+      </c>
+      <c r="G25" s="104"/>
+      <c r="H25" s="161"/>
+      <c r="I25" s="161"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="97"/>
-      <c r="C26" s="97"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="137"/>
       <c r="D26" s="35"/>
       <c r="E26" s="83"/>
       <c r="F26" s="83"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="182"/>
-      <c r="I26" s="182"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="161"/>
+      <c r="I26" s="161"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="97"/>
-      <c r="C27" s="173" t="s">
-        <v>35</v>
+      <c r="B27" s="137"/>
+      <c r="C27" s="183" t="s">
+        <v>37</v>
       </c>
       <c r="D27" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="166">
+      <c r="E27" s="149">
         <f>E31*E29</f>
-        <v>144</v>
-      </c>
-      <c r="F27" s="167">
+        <v>707.59999999999991</v>
+      </c>
+      <c r="F27" s="150">
         <f>G27-E27</f>
-        <v>420</v>
-      </c>
-      <c r="G27" s="170">
-        <v>564</v>
-      </c>
-      <c r="H27" s="182">
+        <v>3689.4</v>
+      </c>
+      <c r="G27" s="152">
+        <v>4397</v>
+      </c>
+      <c r="H27" s="161">
         <f>(E27/F27)/(E28/F28)</f>
-        <v>3.8095238095238098</v>
-      </c>
-      <c r="I27" s="182"/>
+        <v>3.8119871671668708</v>
+      </c>
+      <c r="I27" s="161"/>
       <c r="J27" s="1">
         <f>(E27/(E27+F27))/(E28/(E28+F28))</f>
-        <v>3.0921985815602833</v>
+        <v>3.3594599623710377</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="97"/>
-      <c r="C28" s="174"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="84">
+      <c r="E28" s="136">
         <f>E29-E27</f>
-        <v>36</v>
-      </c>
-      <c r="F28" s="168">
+        <v>268.39999999999998</v>
+      </c>
+      <c r="F28" s="151">
         <f>G28-E28</f>
-        <v>400</v>
-      </c>
-      <c r="G28" s="170">
+        <v>5334.6</v>
+      </c>
+      <c r="G28" s="152">
         <f>G29-G27</f>
-        <v>436</v>
-      </c>
-      <c r="H28" s="182"/>
-      <c r="I28" s="182"/>
+        <v>5603</v>
+      </c>
+      <c r="H28" s="161">
+        <f>(E27/E28)/(F27/F28)</f>
+        <v>3.8119871671668708</v>
+      </c>
+      <c r="I28" s="161"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="97"/>
-      <c r="C29" s="174"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="162">
+      <c r="E29" s="145">
         <f>E30*G29</f>
-        <v>180</v>
-      </c>
-      <c r="F29" s="165">
+        <v>975.99999999999989</v>
+      </c>
+      <c r="F29" s="148">
         <f>F30*G29</f>
-        <v>820.00000000000011</v>
-      </c>
-      <c r="G29" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
+        <v>9024</v>
+      </c>
+      <c r="G29" s="152">
+        <v>10000</v>
+      </c>
+      <c r="H29" s="161"/>
+      <c r="I29" s="161"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="97"/>
+      <c r="B30" s="137"/>
       <c r="C30" s="46"/>
-      <c r="D30" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E30" s="161">
-        <f>(0.5*E46)+(0.5*E54)</f>
-        <v>0.18</v>
-      </c>
-      <c r="F30" s="163">
+      <c r="D30" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="189">
+        <f>E39/100</f>
+        <v>9.7599999999999992E-2</v>
+      </c>
+      <c r="F30" s="146">
         <f>1-E30</f>
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="G30" s="105"/>
-      <c r="H30" s="182"/>
-      <c r="I30" s="182"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="97"/>
-      <c r="C31" s="172"/>
-      <c r="D31" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="183">
-        <v>0.8</v>
-      </c>
-      <c r="F31" s="164">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G30" s="104"/>
+      <c r="H30" s="161"/>
+      <c r="I30" s="161"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="138"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="190">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F31" s="157">
         <f>F27/F29</f>
-        <v>0.51219512195121941</v>
-      </c>
-      <c r="G31" s="105"/>
-      <c r="H31" s="182"/>
-      <c r="I31" s="182"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="182"/>
-      <c r="I32" s="182"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="97"/>
-      <c r="C33" s="173" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="166">
-        <f>E37*E35</f>
-        <v>185.65000000000003</v>
-      </c>
-      <c r="F33" s="167">
-        <f>G33-E33</f>
-        <v>378.34999999999997</v>
-      </c>
-      <c r="G33" s="170">
-        <v>564</v>
-      </c>
-      <c r="H33" s="182">
-        <f>(E33/F33)/(E34/F34)</f>
-        <v>3.8444310194012865</v>
-      </c>
-      <c r="I33" s="182"/>
-      <c r="J33" s="1">
-        <f>(E33/(E33+F33))/(E34/(E34+F34))</f>
-        <v>2.9081391421816964</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="97"/>
-      <c r="C34" s="174"/>
-      <c r="D34" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="84">
-        <f>E35-E33</f>
-        <v>49.349999999999994</v>
-      </c>
-      <c r="F34" s="168">
-        <f>G34-E34</f>
-        <v>386.65</v>
-      </c>
-      <c r="G34" s="170">
-        <f>G35-G33</f>
-        <v>436</v>
-      </c>
-      <c r="H34" s="182"/>
-      <c r="I34" s="182"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="97"/>
-      <c r="C35" s="174"/>
-      <c r="D35" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="162">
-        <f>E36*G35</f>
-        <v>235.00000000000003</v>
-      </c>
-      <c r="F35" s="165">
-        <f>F36*G35</f>
-        <v>765</v>
-      </c>
-      <c r="G35" s="170">
-        <v>1000</v>
-      </c>
-      <c r="H35" s="182"/>
-      <c r="I35" s="182"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="97"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="161">
-        <f>(0.5*E47)+(0.5*E55)</f>
-        <v>0.23500000000000001</v>
-      </c>
-      <c r="F36" s="163">
-        <f>1-E36</f>
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="G36" s="105"/>
-      <c r="H36" s="182"/>
-      <c r="I36" s="182"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="49"/>
-      <c r="C37" s="176"/>
-      <c r="D37" s="109" t="s">
-        <v>120</v>
-      </c>
-      <c r="E37" s="184">
-        <v>0.79</v>
-      </c>
-      <c r="F37" s="177">
-        <f>F33/F35</f>
-        <v>0.49457516339869279</v>
-      </c>
-      <c r="G37" s="175"/>
-      <c r="H37" s="182"/>
-      <c r="I37" s="182"/>
-    </row>
-    <row r="38" spans="2:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J38" s="28"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+        <v>0.40884308510638301</v>
+      </c>
+      <c r="G31" s="155"/>
+      <c r="H31" s="161"/>
+      <c r="I31" s="161"/>
+    </row>
+    <row r="32" spans="2:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C34" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="157" t="s">
-        <v>102</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="156">
-        <v>0.08</v>
-      </c>
-      <c r="F42" s="158" t="s">
+      <c r="D34" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="141" t="s">
+        <v>95</v>
+      </c>
+      <c r="I34" s="152"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="140">
+        <v>0</v>
+      </c>
+      <c r="E35" s="186">
+        <f>D35*100/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="142">
+        <v>0</v>
+      </c>
+      <c r="I35" s="152"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="46"/>
+      <c r="C36" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="140">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E36" s="186">
+        <f t="shared" ref="E36:E39" si="0">D36*100/1000</f>
+        <v>0.5099999999999999</v>
+      </c>
+      <c r="F36" s="142" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="28"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="146" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="156">
-        <v>0.12</v>
-      </c>
-      <c r="F43" s="158" t="s">
-        <v>105</v>
-      </c>
-      <c r="G43" s="28"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="146"/>
-      <c r="C44" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="156">
-        <v>0.12</v>
-      </c>
-      <c r="F44" s="158" t="s">
-        <v>106</v>
-      </c>
-      <c r="G44" s="28"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="146"/>
-      <c r="C45" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="156">
-        <v>0.16</v>
-      </c>
-      <c r="F45" s="158" t="s">
-        <v>104</v>
-      </c>
-      <c r="G45" s="28"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="146"/>
-      <c r="C46" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="156">
-        <v>0.18</v>
-      </c>
-      <c r="F46" s="158" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="28"/>
-    </row>
-    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="147"/>
-      <c r="C47" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="78"/>
-      <c r="E47" s="159">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F47" s="160" t="s">
-        <v>108</v>
-      </c>
-      <c r="G47" s="28"/>
-    </row>
-    <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="111" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="72"/>
-      <c r="E49" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="157" t="s">
-        <v>102</v>
-      </c>
-      <c r="G49" s="28"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="156">
-        <v>0.1</v>
-      </c>
-      <c r="F50" s="158" t="s">
+      <c r="I36" s="152"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="175" t="s">
         <v>110</v>
       </c>
-      <c r="G50" s="28"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="146" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="156">
-        <v>0.11</v>
-      </c>
-      <c r="F51" s="158" t="s">
+      <c r="C37" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="G51" s="28"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="146"/>
-      <c r="C52" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="156">
-        <v>0.06</v>
-      </c>
-      <c r="F52" s="158" t="s">
+      <c r="D37" s="140">
+        <v>14.5</v>
+      </c>
+      <c r="E37" s="186">
+        <f t="shared" si="0"/>
+        <v>1.45</v>
+      </c>
+      <c r="F37" s="142" t="s">
         <v>112</v>
       </c>
-      <c r="G52" s="28"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="146"/>
-      <c r="C53" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="35"/>
-      <c r="E53" s="156">
-        <v>0.12</v>
-      </c>
-      <c r="F53" s="158" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="28"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="146"/>
-      <c r="C54" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="156">
-        <v>0.18</v>
-      </c>
-      <c r="F54" s="158" t="s">
-        <v>107</v>
-      </c>
-      <c r="G54" s="28"/>
-    </row>
-    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="147"/>
-      <c r="C55" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55" s="78"/>
-      <c r="E55" s="159">
-        <v>0.19</v>
-      </c>
-      <c r="F55" s="160" t="s">
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="175"/>
+      <c r="C38" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="G55" s="28"/>
+      <c r="D38" s="140">
+        <v>41.3</v>
+      </c>
+      <c r="E38" s="186">
+        <f t="shared" si="0"/>
+        <v>4.13</v>
+      </c>
+      <c r="F38" s="142" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="176"/>
+      <c r="C39" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="143">
+        <v>97.6</v>
+      </c>
+      <c r="E39" s="187">
+        <f t="shared" si="0"/>
+        <v>9.76</v>
+      </c>
+      <c r="F39" s="144" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C21:C23"/>
+  <mergeCells count="6">
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10574,7 +10306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T14"/>
   <sheetViews>
@@ -10607,43 +10339,43 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="128" t="s">
+      <c r="H3" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="128" t="s">
+      <c r="I3" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="128" t="s">
+      <c r="J3" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="128" t="s">
+      <c r="K3" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="128" t="s">
+      <c r="L3" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="128" t="s">
+      <c r="M3" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="128" t="s">
+      <c r="N3" s="126" t="s">
         <v>85</v>
       </c>
     </row>
@@ -10660,13 +10392,13 @@
       <c r="E4" s="1">
         <v>0.6</v>
       </c>
-      <c r="F4" s="130" t="s">
+      <c r="F4" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="131" t="s">
+      <c r="G4" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="130" t="s">
+      <c r="H4" s="128" t="s">
         <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -10701,10 +10433,10 @@
       <c r="E5" s="1">
         <v>0.6</v>
       </c>
-      <c r="F5" s="130" t="s">
+      <c r="F5" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="131" t="s">
+      <c r="G5" s="129" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -10742,10 +10474,10 @@
       <c r="E6" s="1">
         <v>0.6</v>
       </c>
-      <c r="F6" s="130" t="s">
+      <c r="F6" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="129" t="s">
         <v>83</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -10783,10 +10515,10 @@
       <c r="E7" s="1">
         <v>0.6</v>
       </c>
-      <c r="F7" s="130" t="s">
+      <c r="F7" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="129" t="s">
         <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -10827,56 +10559,56 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:20" s="127" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="128" t="s">
+    <row r="10" spans="2:20" s="125" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="128" t="s">
+      <c r="D10" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="128" t="s">
+      <c r="E10" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="128" t="s">
+      <c r="F10" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="128" t="s">
+      <c r="G10" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="128" t="s">
+      <c r="H10" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="128" t="s">
+      <c r="I10" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="128" t="s">
+      <c r="J10" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="128" t="s">
+      <c r="K10" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="128" t="s">
+      <c r="L10" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="128" t="s">
+      <c r="M10" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="N10" s="128" t="s">
+      <c r="N10" s="126" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="127" t="s">
+      <c r="Q10" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="R10" s="129">
+      <c r="R10" s="127">
         <v>1</v>
       </c>
-      <c r="S10" s="126" t="s">
+      <c r="S10" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="T10" s="126" t="s">
+      <c r="T10" s="124" t="s">
         <v>65</v>
       </c>
     </row>
@@ -10893,13 +10625,13 @@
       <c r="E11" s="1">
         <v>0.6</v>
       </c>
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="131" t="s">
+      <c r="G11" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="130" t="s">
+      <c r="H11" s="128" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -10943,10 +10675,10 @@
       <c r="E12" s="1">
         <v>0.6</v>
       </c>
-      <c r="F12" s="130" t="s">
+      <c r="F12" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="130" t="s">
+      <c r="G12" s="128" t="s">
         <v>84</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -10993,10 +10725,10 @@
       <c r="E13" s="1">
         <v>0.6</v>
       </c>
-      <c r="F13" s="130" t="s">
+      <c r="F13" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="130" t="s">
+      <c r="G13" s="128" t="s">
         <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -11034,10 +10766,10 @@
       <c r="E14" s="1">
         <v>0.6</v>
       </c>
-      <c r="F14" s="130" t="s">
+      <c r="F14" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="130" t="s">
+      <c r="G14" s="128" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="1" t="s">

</xml_diff>